<commit_message>
Update template to solve CURL problem
</commit_message>
<xml_diff>
--- a/data/Liberation_Price Tracker SKU list_v1_Pampers.xlsx
+++ b/data/Liberation_Price Tracker SKU list_v1_Pampers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kang.y.5\OneDrive - Procter and Gamble\Documents\GitHub\liberation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{17BCC08E-1F5D-4046-8FCF-30AF4568CA99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{25D00A97-704C-4765-A569-9113D7AAF760}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="8_{17BCC08E-1F5D-4046-8FCF-30AF4568CA99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{877B6FAB-9E00-409C-AAB5-780CC33C6F76}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="779" xr2:uid="{082D8A25-05B0-4134-80F4-C81249D6F8B7}"/>
   </bookViews>
@@ -40,22 +40,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2101" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="780">
   <si>
     <t>No</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Category</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Brand</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Barcode</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>FR</t>
@@ -95,7 +95,7 @@
   </si>
   <si>
     <t>Priority</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>FA 370</t>
@@ -171,79 +171,79 @@
   </si>
   <si>
     <t>Competitor-1</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Basic Info</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Naver Price Checker site</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Price_Max</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Product Code_NV</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Product Name_NV</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>URL_NV</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Volume_Per_Unit_NV</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>VB_Units_NV</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Product Code_CP</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Item_ID_CP</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Seller_CP</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Product Name_CP</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>URL_CP</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Volume_Per_Unit_CP</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>VB_Units_CP</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Manufacturer</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Coupang (Rocket Delivery - Coupang as Seller)</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>P&amp;G</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Proshield Yellow Blade 8ct</t>
@@ -322,7 +322,7 @@
   </si>
   <si>
     <t>Segment</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>4902430651196</t>
@@ -392,11 +392,11 @@
   </si>
   <si>
     <t>Product Name_En</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Product Name_KR</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>퓨전 프로쉴드 옐로우 면도날 8입</t>
@@ -439,58 +439,58 @@
   </si>
   <si>
     <t>optional</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Optional</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Project Leberation - Product Master File</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Note</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>*# of bottles/ packs in virtual bundling</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>*ml or # of blades/ brushes/ pads</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Go to Naver Price Checker site, and capture the necessary information for in-scope products</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Naver Price Checker site - how to capture necessary information</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Coupang - how to capture necessary information</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>"https://search.shopping.naver.com/detail/detail.nhn?nvMid=" + "Product Code in Naver"</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>*Price Strategy range (Min/Max) for Coupang SKU</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Competitor-2 (Optional - if needed for your category)</t>
   </si>
   <si>
     <t>Competitor-2</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Alerting if the price is out of the range</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>1. Make sure all columns (except for "Optional") are filled. Otherwise, the data will not be accurately tracked.</t>
@@ -509,47 +509,47 @@
   </si>
   <si>
     <t>Naver_Product_Code</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Price</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Shipping_Fee</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>NAVER Price Tracking Transaction Output</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>LP_URL</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Mall_Name</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Seller_Name</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Price_Ranking</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Product_Name</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>*outside of Naver mall: unknown</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>P&amp;G</t>
@@ -1459,87 +1459,87 @@
   </si>
   <si>
     <t>NV_ProductCode</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>NV_ProductName</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>NV_URL</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>NV_Volume_Per_Unit</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>ml</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>NV_VolumeType</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>piece</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>V_VB_Units</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>CP_ProductCode</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>CP_Item_ID</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>CP_Seller</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>CP_ProductName</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>CP_URL</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>CP_Volume_Per_Unit</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>CP_VB_Units</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>CP_PriceMin</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>CP_PriceMax</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>CP_VolumeType</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>ProductName_En</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>ProductName_KR</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>https://www.coupang.com/vp/products/1652632305?itemId=4011670917</t>
-    <phoneticPr fontId="4"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Lager IDD 2.8L</t>
@@ -3854,6 +3854,969 @@
   --compressed</t>
   </si>
   <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/6197001049/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=1440&amp;nvMid=6197001049&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042359&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/6197001049?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=221844|kh44u848|395aa407aa9c951d73d8de3fa3ce656c5d6ef428|s_1a7f4dd73489|97a684e827d8975db0e10abff1118b51d7a85ffa:1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:845657|kh45wqow|5cad2ef28fafd769103a495fa86c4510ccd30c82|s_54853016347d|9e6dc8c0e97a9ab511f0b55a0ba1cd5db2522760:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:24|kh46h9w0|514e6e49616c349dc94d31b9a85cd9a43485113d|s_419afe53a6bb|1f0c44bb64e6ca64f62753fde0a6e9a30d925da0:17703|kh5yj708|1b94217d27ff92d18e091e4b26be526631f2b666|s_1f0b6dd345b2|8da79206b3c0d93283e34b5f8e2e5540b8a420ff:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:692492|kheq2nlc|14e7f0c8a5cb417eecc3ba4821698bd8fdcd3b64|s_a072289e9d4f|414aa3c087e4b7cefb044f78174600558dc93cf7' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/7334104980/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=1150&amp;nvMid=7334104980&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042359&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/7334104980?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=221844|kh44u848|395aa407aa9c951d73d8de3fa3ce656c5d6ef428|s_1a7f4dd73489|97a684e827d8975db0e10abff1118b51d7a85ffa:1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:845657|kh45wqow|5cad2ef28fafd769103a495fa86c4510ccd30c82|s_54853016347d|9e6dc8c0e97a9ab511f0b55a0ba1cd5db2522760:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:24|kh46h9w0|514e6e49616c349dc94d31b9a85cd9a43485113d|s_419afe53a6bb|1f0c44bb64e6ca64f62753fde0a6e9a30d925da0:17703|kh5yj708|1b94217d27ff92d18e091e4b26be526631f2b666|s_1f0b6dd345b2|8da79206b3c0d93283e34b5f8e2e5540b8a420ff:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:692492|kheq2nlc|14e7f0c8a5cb417eecc3ba4821698bd8fdcd3b64|s_a072289e9d4f|414aa3c087e4b7cefb044f78174600558dc93cf7' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/23684181490/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=9850&amp;nvMid=23684181490&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042364&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/23684181490?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=221844|kh44u848|395aa407aa9c951d73d8de3fa3ce656c5d6ef428|s_1a7f4dd73489|97a684e827d8975db0e10abff1118b51d7a85ffa:1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:24|kh46h9w0|514e6e49616c349dc94d31b9a85cd9a43485113d|s_419afe53a6bb|1f0c44bb64e6ca64f62753fde0a6e9a30d925da0:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:692492|kheq2nlc|14e7f0c8a5cb417eecc3ba4821698bd8fdcd3b64|s_a072289e9d4f|414aa3c087e4b7cefb044f78174600558dc93cf7:17703|kheqmswg|8cb186da6ded016ac94de23a7b59459338fd964e|s_1f0b6dd345b2|df5defae78211a3108a57f81d7924f069d7cc73e:845657|kheqmwrc|22064414ff140b36d4150fd78f93604d2672ebf3|s_54853016347d|20eeeaebf2e1a61a5de0dbc0c3c733139f9eeaa3' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/13396543418/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=7340&amp;nvMid=13396543418&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013179&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/13396543418?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:17703|kheqmswg|8cb186da6ded016ac94de23a7b59459338fd964e|s_1f0b6dd345b2|df5defae78211a3108a57f81d7924f069d7cc73e:845657|kheqmwrc|22064414ff140b36d4150fd78f93604d2672ebf3|s_54853016347d|20eeeaebf2e1a61a5de0dbc0c3c733139f9eeaa3:24|kheqpcq0|7e207eebac55b8ef235f1479ce4eece48d1015d6|s_419afe53a6bb|56e078d4d28e36eb9a7a4f0b37cc568aabd84835:3|kheqprds|ddd7765f03280b8258132237c4bd239496df224a|s_22aec0678481|cfe1be17a573ad63634c691fe5b075e8f9620336:692492|kheqq8cw|51de67d1db6cbd9120df8a6c67e76e66d0705b4c|s_a072289e9d4f|aa955c9604f03fd49fffecdfe06c82e201f1f2ed' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/18621865118/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=16990&amp;nvMid=18621865118&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013181&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/18621865118?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:17703|kheqmswg|8cb186da6ded016ac94de23a7b59459338fd964e|s_1f0b6dd345b2|df5defae78211a3108a57f81d7924f069d7cc73e:845657|kheqmwrc|22064414ff140b36d4150fd78f93604d2672ebf3|s_54853016347d|20eeeaebf2e1a61a5de0dbc0c3c733139f9eeaa3:3|kheqprds|ddd7765f03280b8258132237c4bd239496df224a|s_22aec0678481|cfe1be17a573ad63634c691fe5b075e8f9620336:692492|kheqq8cw|51de67d1db6cbd9120df8a6c67e76e66d0705b4c|s_a072289e9d4f|aa955c9604f03fd49fffecdfe06c82e201f1f2ed:24|kheqv6lk|6bd7de86cc096c09ad2c0c3b86122efd721c6aab|s_419afe53a6bb|144ae6041b1acd909e30990b156e1d401cc57c58:1256411|kheqvb88|92f277c1550a5cbef08de00112a55a7225e119f5|s_3108672e8f2f6|aaf926b15c97c968f023b1aa11692f01575ccc33' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/23692847497/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=10690&amp;nvMid=23692847497&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013181&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/23692847497?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:17703|kheqmswg|8cb186da6ded016ac94de23a7b59459338fd964e|s_1f0b6dd345b2|df5defae78211a3108a57f81d7924f069d7cc73e:845657|kheqmwrc|22064414ff140b36d4150fd78f93604d2672ebf3|s_54853016347d|20eeeaebf2e1a61a5de0dbc0c3c733139f9eeaa3:3|kheqprds|ddd7765f03280b8258132237c4bd239496df224a|s_22aec0678481|cfe1be17a573ad63634c691fe5b075e8f9620336:692492|kheqq8cw|51de67d1db6cbd9120df8a6c67e76e66d0705b4c|s_a072289e9d4f|aa955c9604f03fd49fffecdfe06c82e201f1f2ed:24|kheqv6lk|6bd7de86cc096c09ad2c0c3b86122efd721c6aab|s_419afe53a6bb|144ae6041b1acd909e30990b156e1d401cc57c58:1256411|kheqvb88|92f277c1550a5cbef08de00112a55a7225e119f5|s_3108672e8f2f6|aaf926b15c97c968f023b1aa11692f01575ccc33:1243359|kheqygnk|0333fe04836d77eba328521fa137ee68a6208015|s_20e2dda6a19a|28e17b8496daa02c1d7381cc309dc083be576119:199209|kheqyiyw|dce533f2a5e494d7477481645d542735314fbe2e|s_3983c5348f46f5f1|2b2ca89b5658c4c9758b12f75d362ac50c383ea6' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/23379646490/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=13940&amp;nvMid=23379646490&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/23379646490?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/18620494198/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=11110&amp;nvMid=18620494198&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013186&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/18620494198?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/23378976493/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=9830&amp;nvMid=23378976493&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/23378976493?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21033910311/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=15400&amp;nvMid=21033910311&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21033910311?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21032565501/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=11900&amp;nvMid=21032565501&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21032565501?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21032656061/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=8800&amp;nvMid=21032656061&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21032656061?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21032592926/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=8850&amp;nvMid=21032592926&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21032592926?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21033910847/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=15400&amp;nvMid=21033910847&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21033910847?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21833037524/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=8750&amp;nvMid=21833037524&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21833037524?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>Babydry Pants S3</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 팬티 3단계(중형) 46X4</t>
+  </si>
+  <si>
+    <t>14902430671672</t>
+  </si>
+  <si>
+    <t>Baby</t>
+  </si>
+  <si>
+    <t>Pampers</t>
+  </si>
+  <si>
+    <t>Pants</t>
+  </si>
+  <si>
+    <t>Babydry Pants S4</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 팬티 4단계(대형) 42X4</t>
+  </si>
+  <si>
+    <t>14902430671689</t>
+  </si>
+  <si>
+    <t>Babydry Pants S5</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 팬티 5단계(특대형) 36X4</t>
+  </si>
+  <si>
+    <t>14902430671696</t>
+  </si>
+  <si>
+    <t>Babydry Pants S6</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 팬티 6단계(점보형) 28X4</t>
+  </si>
+  <si>
+    <t>14902430671702</t>
+  </si>
+  <si>
+    <t>Overnight Pants S4</t>
+  </si>
+  <si>
+    <t>팸퍼스 통잠팬티 4단계 30 X 4</t>
+  </si>
+  <si>
+    <t>14902430897058</t>
+  </si>
+  <si>
+    <t>Overnight Pants S5</t>
+  </si>
+  <si>
+    <t>팸퍼스 통잠팬티 5단계 26 X 4</t>
+  </si>
+  <si>
+    <t>14902430897065</t>
+  </si>
+  <si>
+    <t>Overnight Pants S6</t>
+  </si>
+  <si>
+    <t>팸퍼스 통잠팬티 6단계 22 X 4</t>
+  </si>
+  <si>
+    <t>14902430897072</t>
+  </si>
+  <si>
+    <t>Babydry Tape S2</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 2단계 이노머스 박스 1/186</t>
+  </si>
+  <si>
+    <t>037000783794</t>
+  </si>
+  <si>
+    <t>Tape</t>
+  </si>
+  <si>
+    <t>Babydry Tape S3</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이3단계 이노머스 박스1/168</t>
+  </si>
+  <si>
+    <t>037000783800</t>
+  </si>
+  <si>
+    <t>Babydry Tape S4</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 4단계 이노머스 박스 1/150</t>
+  </si>
+  <si>
+    <t>037000783817</t>
+  </si>
+  <si>
+    <t>Babydry Tape S5</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 5단계 이노머스 박스 1/132</t>
+  </si>
+  <si>
+    <t>037000783824</t>
+  </si>
+  <si>
+    <t>Babydry Tape S6</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 6단계 이노머스 박스 1/112</t>
+  </si>
+  <si>
+    <t>037000783831</t>
+  </si>
+  <si>
+    <t>Swaddlers Tape S1</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 1단계 32X4</t>
+  </si>
+  <si>
+    <t>10037000749568</t>
+  </si>
+  <si>
+    <t>Swaddlers Tape S2</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 2단계 29X4</t>
+  </si>
+  <si>
+    <t>10037000749605</t>
+  </si>
+  <si>
+    <t>Swaddlers Tape S3</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 3단계 26X4</t>
+  </si>
+  <si>
+    <t>10037000748974</t>
+  </si>
+  <si>
+    <t>Swaddlers Tape S4</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 4단계 22X4</t>
+  </si>
+  <si>
+    <t>10037000749582</t>
+  </si>
+  <si>
+    <t>Swaddlers Tape S5</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 5단계 19X4</t>
+  </si>
+  <si>
+    <t>10037000749599</t>
+  </si>
+  <si>
+    <t>Swaddlers Tape S6</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 6단계 16X4</t>
+  </si>
+  <si>
+    <t>10037000749612</t>
+  </si>
+  <si>
+    <t>팸퍼스 2016 베이비드라이 3단계 팬티형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=9606247018</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비 드라이 기저귀 4단계 팬티형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21798278124</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비 드라이 기저귀 5단계 팬티형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=20804055294</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비 드라이 기저귀 6단계 팬티형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=20804087696</t>
+  </si>
+  <si>
+    <t>팸퍼스 통잠팬티 기저귀 4단계 팬티형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=24355155523</t>
+  </si>
+  <si>
+    <t>팸퍼스 통잠팬티 기저귀 5단계 팬티형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=24355221522</t>
+  </si>
+  <si>
+    <t>팸퍼스 통잠팬티 기저귀 6-7단계 팬티형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=24355278522</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비 드라이 기저귀 2단계 밴드형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21800768787</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비 드라이 기저귀 3단계 밴드형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21800772029</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비 드라이 기저귀 4단계 밴드형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21799603401</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비 드라이 기저귀 5단계 밴드형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21799480376</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비 드라이 기저귀 6단계 밴드형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21800790512</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 기저귀 1단계 밴드형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21793228443</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 기저귀 2단계 밴드형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21793256416</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 기저귀 3단계 밴드형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21793256419</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 기저귀 4단계 밴드형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21968910906</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 기저귀 5단계 밴드형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21793284456</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 기저귀 6단계 밴드형</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=23399582505</t>
+  </si>
+  <si>
+    <t>1474384</t>
+  </si>
+  <si>
+    <t>6449086</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 팬티형 기저귀 아동공용 M 3단계 (7~12kg)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/1474384?itemId=6449086</t>
+  </si>
+  <si>
+    <t>1474385</t>
+  </si>
+  <si>
+    <t>6449087</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 팬티형 기저귀 아동공용 L 4단계 (9~14kg)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/1474385?itemId=6449087</t>
+  </si>
+  <si>
+    <t>1474386</t>
+  </si>
+  <si>
+    <t>6449088</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비 드라이 팬티형 기저귀 아동공용 특대형 5단계(12~17kg)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/1474386?itemId=6449088</t>
+  </si>
+  <si>
+    <t>2387028</t>
+  </si>
+  <si>
+    <t>10975373</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 팬티형 기저귀 XXL 6단계(15~25kg)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/2387028?itemId=10975373</t>
+  </si>
+  <si>
+    <t>2129373823</t>
+  </si>
+  <si>
+    <t>3614045491</t>
+  </si>
+  <si>
+    <t>팸퍼스 통잠 팬티형 기저귀 아동용 4단계(9~14kg) 4p</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/2129373823?itemId=3614045491</t>
+  </si>
+  <si>
+    <t>2129373940</t>
+  </si>
+  <si>
+    <t>3614045651</t>
+  </si>
+  <si>
+    <t>팸퍼스 통잠 팬티형 기저귀 아동용 5단계(12~17kg) 4p</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/2129373940?itemId=3614045651</t>
+  </si>
+  <si>
+    <t>2129373882</t>
+  </si>
+  <si>
+    <t>3614045563</t>
+  </si>
+  <si>
+    <t>팸퍼스 통잠 팬티형 기저귀 아동용 6-7단계(15~25kg) 4p</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/2129373882?itemId=3614045563</t>
+  </si>
+  <si>
+    <t>198248953</t>
+  </si>
+  <si>
+    <t>572284449</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 이노머스팩 밴드형 기저귀 아동공용 2단계(4~6kg)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/198248953?itemId=572284449</t>
+  </si>
+  <si>
+    <t>203384751</t>
+  </si>
+  <si>
+    <t>596704427</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 밴드형 기저귀 아동공용 3단계(7~13kg)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/203384751?itemId=596704427</t>
+  </si>
+  <si>
+    <t>324536335</t>
+  </si>
+  <si>
+    <t>1038931487</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 밴드형 기저귀 아동공용 4단계(10~17kg)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/324536335?itemId=1038931487</t>
+  </si>
+  <si>
+    <t>324537029</t>
+  </si>
+  <si>
+    <t>1038933819</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 밴드형 기저귀 아동공용 5단계 (12kg~)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/324537029?itemId=1038933819</t>
+  </si>
+  <si>
+    <t>284947230</t>
+  </si>
+  <si>
+    <t>904172543</t>
+  </si>
+  <si>
+    <t>팸퍼스 베이비드라이 밴드형 기저귀 이노머스팩 6단계(16kg~)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/284947230?itemId=904172543</t>
+  </si>
+  <si>
+    <t>174663237</t>
+  </si>
+  <si>
+    <t>498913162</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 밴드형 기저귀 아동공용 1단계(4~6kg)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/174663237?itemId=498913162</t>
+  </si>
+  <si>
+    <t>174683312</t>
+  </si>
+  <si>
+    <t>499046748</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 밴드형 기저귀 아동공용 2단계(5~8kg)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/174683312?itemId=499046748</t>
+  </si>
+  <si>
+    <t>174683311</t>
+  </si>
+  <si>
+    <t>499046739</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 밴드형 기저귀 아동공용 3단계(7~13kg)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/174683311?itemId=499046739</t>
+  </si>
+  <si>
+    <t>174683303</t>
+  </si>
+  <si>
+    <t>499046695</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 밴드형 기저귀 아동공용 4단계(10~17kg)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/174683303?itemId=499046695</t>
+  </si>
+  <si>
+    <t>174683688</t>
+  </si>
+  <si>
+    <t>499049033</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 밴드형 기저귀 아동공용 5단계(12kg~)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/174683688?itemId=499049033</t>
+  </si>
+  <si>
+    <t>174662956</t>
+  </si>
+  <si>
+    <t>498912308</t>
+  </si>
+  <si>
+    <t>팸퍼스 스와들러 밴드형 기저귀 6단계(16kg~)</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/174662956?itemId=498912308</t>
+  </si>
+  <si>
+    <t>ea</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/9606247018/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=52150&amp;nvMid=9606247018&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043098&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/9606247018?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21798278124/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=51070&amp;nvMid=21798278124&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042987&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21798278124?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/20804055294/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=51600&amp;nvMid=20804055294&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042994&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/20804055294?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/20804087696/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=53760&amp;nvMid=20804087696&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043009&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/20804087696?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/24355155523/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=39040&amp;nvMid=24355155523&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043013&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=DEFAULT&amp;inflow=slc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/24355155523?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/24355221522/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=39040&amp;nvMid=24355221522&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042980&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=DEFAULT&amp;inflow=slc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/24355221522?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/24355278522/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=39040&amp;nvMid=24355278522&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043044&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=DEFAULT&amp;inflow=slc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/24355278522?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21800768787/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=49900&amp;nvMid=21800768787&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043007&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21800768787?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21800772029/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=49870&amp;nvMid=21800772029&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042987&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21800772029?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21799603401/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=40960&amp;nvMid=21799603401&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043032&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21799603401?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21799480376/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=40960&amp;nvMid=21799480376&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043053&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21799480376?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21800790512/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=41870&amp;nvMid=21800790512&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043009&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21800790512?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21793228443/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=30830&amp;nvMid=21793228443&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043002&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21793228443?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21793256416/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=29110&amp;nvMid=21793256416&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043069&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21793256416?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21793256419/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=38940&amp;nvMid=21793256419&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042980&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21793256419?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21968910906/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=30100&amp;nvMid=21968910906&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043044&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21968910906?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21793284456/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=29110&amp;nvMid=21793284456&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043052&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21793284456?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/23399582505/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=30400&amp;nvMid=23399582505&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043036&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/23399582505?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
     <t>curl 'https://search.shopping.naver.com/catalog/9768921714/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=1380&amp;nvMid=9768921714&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042359&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
   -H 'Connection: keep-alive' \
   -H 'Accept: application/json, text/plain, */*' \
@@ -3867,983 +4830,6 @@
   -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=221844|kh44u848|395aa407aa9c951d73d8de3fa3ce656c5d6ef428|s_1a7f4dd73489|97a684e827d8975db0e10abff1118b51d7a85ffa:1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:845657|kh45wqow|5cad2ef28fafd769103a495fa86c4510ccd30c82|s_54853016347d|9e6dc8c0e97a9ab511f0b55a0ba1cd5db2522760:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:24|kh46h9w0|514e6e49616c349dc94d31b9a85cd9a43485113d|s_419afe53a6bb|1f0c44bb64e6ca64f62753fde0a6e9a30d925da0:17703|kh5yj708|1b94217d27ff92d18e091e4b26be526631f2b666|s_1f0b6dd345b2|8da79206b3c0d93283e34b5f8e2e5540b8a420ff:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:692492|kheq2nlc|14e7f0c8a5cb417eecc3ba4821698bd8fdcd3b64|s_a072289e9d4f|414aa3c087e4b7cefb044f78174600558dc93cf7' \
   --compressed</t>
   </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/6197001049/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=1440&amp;nvMid=6197001049&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042359&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/6197001049?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=221844|kh44u848|395aa407aa9c951d73d8de3fa3ce656c5d6ef428|s_1a7f4dd73489|97a684e827d8975db0e10abff1118b51d7a85ffa:1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:845657|kh45wqow|5cad2ef28fafd769103a495fa86c4510ccd30c82|s_54853016347d|9e6dc8c0e97a9ab511f0b55a0ba1cd5db2522760:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:24|kh46h9w0|514e6e49616c349dc94d31b9a85cd9a43485113d|s_419afe53a6bb|1f0c44bb64e6ca64f62753fde0a6e9a30d925da0:17703|kh5yj708|1b94217d27ff92d18e091e4b26be526631f2b666|s_1f0b6dd345b2|8da79206b3c0d93283e34b5f8e2e5540b8a420ff:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:692492|kheq2nlc|14e7f0c8a5cb417eecc3ba4821698bd8fdcd3b64|s_a072289e9d4f|414aa3c087e4b7cefb044f78174600558dc93cf7' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/7334104980/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=1150&amp;nvMid=7334104980&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042359&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/7334104980?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=221844|kh44u848|395aa407aa9c951d73d8de3fa3ce656c5d6ef428|s_1a7f4dd73489|97a684e827d8975db0e10abff1118b51d7a85ffa:1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:845657|kh45wqow|5cad2ef28fafd769103a495fa86c4510ccd30c82|s_54853016347d|9e6dc8c0e97a9ab511f0b55a0ba1cd5db2522760:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:24|kh46h9w0|514e6e49616c349dc94d31b9a85cd9a43485113d|s_419afe53a6bb|1f0c44bb64e6ca64f62753fde0a6e9a30d925da0:17703|kh5yj708|1b94217d27ff92d18e091e4b26be526631f2b666|s_1f0b6dd345b2|8da79206b3c0d93283e34b5f8e2e5540b8a420ff:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:692492|kheq2nlc|14e7f0c8a5cb417eecc3ba4821698bd8fdcd3b64|s_a072289e9d4f|414aa3c087e4b7cefb044f78174600558dc93cf7' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/23684181490/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=9850&amp;nvMid=23684181490&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042364&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/23684181490?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=221844|kh44u848|395aa407aa9c951d73d8de3fa3ce656c5d6ef428|s_1a7f4dd73489|97a684e827d8975db0e10abff1118b51d7a85ffa:1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:24|kh46h9w0|514e6e49616c349dc94d31b9a85cd9a43485113d|s_419afe53a6bb|1f0c44bb64e6ca64f62753fde0a6e9a30d925da0:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:692492|kheq2nlc|14e7f0c8a5cb417eecc3ba4821698bd8fdcd3b64|s_a072289e9d4f|414aa3c087e4b7cefb044f78174600558dc93cf7:17703|kheqmswg|8cb186da6ded016ac94de23a7b59459338fd964e|s_1f0b6dd345b2|df5defae78211a3108a57f81d7924f069d7cc73e:845657|kheqmwrc|22064414ff140b36d4150fd78f93604d2672ebf3|s_54853016347d|20eeeaebf2e1a61a5de0dbc0c3c733139f9eeaa3' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/13396543418/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=7340&amp;nvMid=13396543418&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013179&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/13396543418?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:17703|kheqmswg|8cb186da6ded016ac94de23a7b59459338fd964e|s_1f0b6dd345b2|df5defae78211a3108a57f81d7924f069d7cc73e:845657|kheqmwrc|22064414ff140b36d4150fd78f93604d2672ebf3|s_54853016347d|20eeeaebf2e1a61a5de0dbc0c3c733139f9eeaa3:24|kheqpcq0|7e207eebac55b8ef235f1479ce4eece48d1015d6|s_419afe53a6bb|56e078d4d28e36eb9a7a4f0b37cc568aabd84835:3|kheqprds|ddd7765f03280b8258132237c4bd239496df224a|s_22aec0678481|cfe1be17a573ad63634c691fe5b075e8f9620336:692492|kheqq8cw|51de67d1db6cbd9120df8a6c67e76e66d0705b4c|s_a072289e9d4f|aa955c9604f03fd49fffecdfe06c82e201f1f2ed' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/18621865118/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=16990&amp;nvMid=18621865118&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013181&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/18621865118?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:17703|kheqmswg|8cb186da6ded016ac94de23a7b59459338fd964e|s_1f0b6dd345b2|df5defae78211a3108a57f81d7924f069d7cc73e:845657|kheqmwrc|22064414ff140b36d4150fd78f93604d2672ebf3|s_54853016347d|20eeeaebf2e1a61a5de0dbc0c3c733139f9eeaa3:3|kheqprds|ddd7765f03280b8258132237c4bd239496df224a|s_22aec0678481|cfe1be17a573ad63634c691fe5b075e8f9620336:692492|kheqq8cw|51de67d1db6cbd9120df8a6c67e76e66d0705b4c|s_a072289e9d4f|aa955c9604f03fd49fffecdfe06c82e201f1f2ed:24|kheqv6lk|6bd7de86cc096c09ad2c0c3b86122efd721c6aab|s_419afe53a6bb|144ae6041b1acd909e30990b156e1d401cc57c58:1256411|kheqvb88|92f277c1550a5cbef08de00112a55a7225e119f5|s_3108672e8f2f6|aaf926b15c97c968f023b1aa11692f01575ccc33' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/23692847497/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=10690&amp;nvMid=23692847497&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013181&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/23692847497?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:17703|kheqmswg|8cb186da6ded016ac94de23a7b59459338fd964e|s_1f0b6dd345b2|df5defae78211a3108a57f81d7924f069d7cc73e:845657|kheqmwrc|22064414ff140b36d4150fd78f93604d2672ebf3|s_54853016347d|20eeeaebf2e1a61a5de0dbc0c3c733139f9eeaa3:3|kheqprds|ddd7765f03280b8258132237c4bd239496df224a|s_22aec0678481|cfe1be17a573ad63634c691fe5b075e8f9620336:692492|kheqq8cw|51de67d1db6cbd9120df8a6c67e76e66d0705b4c|s_a072289e9d4f|aa955c9604f03fd49fffecdfe06c82e201f1f2ed:24|kheqv6lk|6bd7de86cc096c09ad2c0c3b86122efd721c6aab|s_419afe53a6bb|144ae6041b1acd909e30990b156e1d401cc57c58:1256411|kheqvb88|92f277c1550a5cbef08de00112a55a7225e119f5|s_3108672e8f2f6|aaf926b15c97c968f023b1aa11692f01575ccc33:1243359|kheqygnk|0333fe04836d77eba328521fa137ee68a6208015|s_20e2dda6a19a|28e17b8496daa02c1d7381cc309dc083be576119:199209|kheqyiyw|dce533f2a5e494d7477481645d542735314fbe2e|s_3983c5348f46f5f1|2b2ca89b5658c4c9758b12f75d362ac50c383ea6' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/23379646490/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=13940&amp;nvMid=23379646490&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/23379646490?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/18620494198/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=11110&amp;nvMid=18620494198&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013186&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/18620494198?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/23378976493/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=9830&amp;nvMid=23378976493&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/23378976493?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21033910311/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=15400&amp;nvMid=21033910311&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21033910311?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21032565501/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=11900&amp;nvMid=21032565501&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21032565501?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21032656061/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=8800&amp;nvMid=21032656061&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21032656061?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21032592926/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=8850&amp;nvMid=21032592926&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21032592926?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21033910847/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=15400&amp;nvMid=21033910847&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21033910847?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21833037524/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=8750&amp;nvMid=21833037524&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013176&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.66 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21833037524?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; ssm_au_c=kvugCAJyWf4QFynkKfZebZO1cqSUnDO21tPNyTK+f9DggAAAAgkJj1HUfawG8rPyNZKpy5p/EoT+JyMPBr/0mKzZ3I9M=; NID_SES=AAABoPs0HKisSxKYpv685nsK3K0Xseq9xS+vnVTbHPI9Q7TvyWb9mBNLbPrz2L//q9Xlh+pQZqDSj0R8dLqi7Fsi0jr73oQ+u7Ddhxc285Ng1xUWwKdTGu3H8l5ubolz4GSVNsrq8aV/j68EPktXwQZ6SQnrBzZC5YmGbLGkODtOMTUg4zNEt3zdDxn7xmhTY/+/ZUb476lR6hY6RKc8QLK56DPaJl/i6J77AlMXm3knz2yxDILk64Mb5fNT9V9nrN4ehHaphCBvDLnRunVN1LDoFZt+CbLDZ7qih1y7lDSGj3OPSLYlwJ5G81dxhOJ4MpUQvYq+xyQLbESS8rDPNVJklspLHMNl985JrAl5+0rk1eAbLrTazQX3tvrBYVRGcysZIEcU6IyJOI61Dkq1w4vHyM/OyBhUsy9LIwvKFgOvqb8aGpq9q+T7L1ligOPRgi3HLaNpsh7uwRpfqBl8V22nTSMynA/7bhFJvs6llT9HWleMpFTMu4EY8XzYptQa7wcy+yMOkaTKhxUtyQ7GiN2LkY8kgV+VuexQ1d24AbZvn5fR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>Babydry Pants S3</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 팬티 3단계(중형) 46X4</t>
-  </si>
-  <si>
-    <t>14902430671672</t>
-  </si>
-  <si>
-    <t>Baby</t>
-  </si>
-  <si>
-    <t>Pampers</t>
-  </si>
-  <si>
-    <t>Pants</t>
-  </si>
-  <si>
-    <t>Babydry Pants S4</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 팬티 4단계(대형) 42X4</t>
-  </si>
-  <si>
-    <t>14902430671689</t>
-  </si>
-  <si>
-    <t>Babydry Pants S5</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 팬티 5단계(특대형) 36X4</t>
-  </si>
-  <si>
-    <t>14902430671696</t>
-  </si>
-  <si>
-    <t>Babydry Pants S6</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 팬티 6단계(점보형) 28X4</t>
-  </si>
-  <si>
-    <t>14902430671702</t>
-  </si>
-  <si>
-    <t>Overnight Pants S4</t>
-  </si>
-  <si>
-    <t>팸퍼스 통잠팬티 4단계 30 X 4</t>
-  </si>
-  <si>
-    <t>14902430897058</t>
-  </si>
-  <si>
-    <t>Overnight Pants S5</t>
-  </si>
-  <si>
-    <t>팸퍼스 통잠팬티 5단계 26 X 4</t>
-  </si>
-  <si>
-    <t>14902430897065</t>
-  </si>
-  <si>
-    <t>Overnight Pants S6</t>
-  </si>
-  <si>
-    <t>팸퍼스 통잠팬티 6단계 22 X 4</t>
-  </si>
-  <si>
-    <t>14902430897072</t>
-  </si>
-  <si>
-    <t>Babydry Tape S2</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 2단계 이노머스 박스 1/186</t>
-  </si>
-  <si>
-    <t>037000783794</t>
-  </si>
-  <si>
-    <t>Tape</t>
-  </si>
-  <si>
-    <t>Babydry Tape S3</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이3단계 이노머스 박스1/168</t>
-  </si>
-  <si>
-    <t>037000783800</t>
-  </si>
-  <si>
-    <t>Babydry Tape S4</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 4단계 이노머스 박스 1/150</t>
-  </si>
-  <si>
-    <t>037000783817</t>
-  </si>
-  <si>
-    <t>Babydry Tape S5</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 5단계 이노머스 박스 1/132</t>
-  </si>
-  <si>
-    <t>037000783824</t>
-  </si>
-  <si>
-    <t>Babydry Tape S6</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 6단계 이노머스 박스 1/112</t>
-  </si>
-  <si>
-    <t>037000783831</t>
-  </si>
-  <si>
-    <t>Swaddlers Tape S1</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 1단계 32X4</t>
-  </si>
-  <si>
-    <t>10037000749568</t>
-  </si>
-  <si>
-    <t>Swaddlers Tape S2</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 2단계 29X4</t>
-  </si>
-  <si>
-    <t>10037000749605</t>
-  </si>
-  <si>
-    <t>Swaddlers Tape S3</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 3단계 26X4</t>
-  </si>
-  <si>
-    <t>10037000748974</t>
-  </si>
-  <si>
-    <t>Swaddlers Tape S4</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 4단계 22X4</t>
-  </si>
-  <si>
-    <t>10037000749582</t>
-  </si>
-  <si>
-    <t>Swaddlers Tape S5</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 5단계 19X4</t>
-  </si>
-  <si>
-    <t>10037000749599</t>
-  </si>
-  <si>
-    <t>Swaddlers Tape S6</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 6단계 16X4</t>
-  </si>
-  <si>
-    <t>10037000749612</t>
-  </si>
-  <si>
-    <t>팸퍼스 2016 베이비드라이 3단계 팬티형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=9606247018</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비 드라이 기저귀 4단계 팬티형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21798278124</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비 드라이 기저귀 5단계 팬티형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=20804055294</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비 드라이 기저귀 6단계 팬티형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=20804087696</t>
-  </si>
-  <si>
-    <t>팸퍼스 통잠팬티 기저귀 4단계 팬티형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=24355155523</t>
-  </si>
-  <si>
-    <t>팸퍼스 통잠팬티 기저귀 5단계 팬티형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=24355221522</t>
-  </si>
-  <si>
-    <t>팸퍼스 통잠팬티 기저귀 6-7단계 팬티형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=24355278522</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비 드라이 기저귀 2단계 밴드형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21800768787</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비 드라이 기저귀 3단계 밴드형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21800772029</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비 드라이 기저귀 4단계 밴드형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21799603401</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비 드라이 기저귀 5단계 밴드형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21799480376</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비 드라이 기저귀 6단계 밴드형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21800790512</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 기저귀 1단계 밴드형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21793228443</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 기저귀 2단계 밴드형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21793256416</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 기저귀 3단계 밴드형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21793256419</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 기저귀 4단계 밴드형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21968910906</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 기저귀 5단계 밴드형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=21793284456</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 기저귀 6단계 밴드형</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=23399582505</t>
-  </si>
-  <si>
-    <t>1474384</t>
-  </si>
-  <si>
-    <t>6449086</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 팬티형 기저귀 아동공용 M 3단계 (7~12kg)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/1474384?itemId=6449086</t>
-  </si>
-  <si>
-    <t>1474385</t>
-  </si>
-  <si>
-    <t>6449087</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 팬티형 기저귀 아동공용 L 4단계 (9~14kg)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/1474385?itemId=6449087</t>
-  </si>
-  <si>
-    <t>1474386</t>
-  </si>
-  <si>
-    <t>6449088</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비 드라이 팬티형 기저귀 아동공용 특대형 5단계(12~17kg)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/1474386?itemId=6449088</t>
-  </si>
-  <si>
-    <t>2387028</t>
-  </si>
-  <si>
-    <t>10975373</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 팬티형 기저귀 XXL 6단계(15~25kg)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/2387028?itemId=10975373</t>
-  </si>
-  <si>
-    <t>2129373823</t>
-  </si>
-  <si>
-    <t>3614045491</t>
-  </si>
-  <si>
-    <t>팸퍼스 통잠 팬티형 기저귀 아동용 4단계(9~14kg) 4p</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/2129373823?itemId=3614045491</t>
-  </si>
-  <si>
-    <t>2129373940</t>
-  </si>
-  <si>
-    <t>3614045651</t>
-  </si>
-  <si>
-    <t>팸퍼스 통잠 팬티형 기저귀 아동용 5단계(12~17kg) 4p</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/2129373940?itemId=3614045651</t>
-  </si>
-  <si>
-    <t>2129373882</t>
-  </si>
-  <si>
-    <t>3614045563</t>
-  </si>
-  <si>
-    <t>팸퍼스 통잠 팬티형 기저귀 아동용 6-7단계(15~25kg) 4p</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/2129373882?itemId=3614045563</t>
-  </si>
-  <si>
-    <t>198248953</t>
-  </si>
-  <si>
-    <t>572284449</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 이노머스팩 밴드형 기저귀 아동공용 2단계(4~6kg)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/198248953?itemId=572284449</t>
-  </si>
-  <si>
-    <t>203384751</t>
-  </si>
-  <si>
-    <t>596704427</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 밴드형 기저귀 아동공용 3단계(7~13kg)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/203384751?itemId=596704427</t>
-  </si>
-  <si>
-    <t>324536335</t>
-  </si>
-  <si>
-    <t>1038931487</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 밴드형 기저귀 아동공용 4단계(10~17kg)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/324536335?itemId=1038931487</t>
-  </si>
-  <si>
-    <t>324537029</t>
-  </si>
-  <si>
-    <t>1038933819</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 밴드형 기저귀 아동공용 5단계 (12kg~)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/324537029?itemId=1038933819</t>
-  </si>
-  <si>
-    <t>284947230</t>
-  </si>
-  <si>
-    <t>904172543</t>
-  </si>
-  <si>
-    <t>팸퍼스 베이비드라이 밴드형 기저귀 이노머스팩 6단계(16kg~)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/284947230?itemId=904172543</t>
-  </si>
-  <si>
-    <t>174663237</t>
-  </si>
-  <si>
-    <t>498913162</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 밴드형 기저귀 아동공용 1단계(4~6kg)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/174663237?itemId=498913162</t>
-  </si>
-  <si>
-    <t>174683312</t>
-  </si>
-  <si>
-    <t>499046748</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 밴드형 기저귀 아동공용 2단계(5~8kg)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/174683312?itemId=499046748</t>
-  </si>
-  <si>
-    <t>174683311</t>
-  </si>
-  <si>
-    <t>499046739</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 밴드형 기저귀 아동공용 3단계(7~13kg)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/174683311?itemId=499046739</t>
-  </si>
-  <si>
-    <t>174683303</t>
-  </si>
-  <si>
-    <t>499046695</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 밴드형 기저귀 아동공용 4단계(10~17kg)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/174683303?itemId=499046695</t>
-  </si>
-  <si>
-    <t>174683688</t>
-  </si>
-  <si>
-    <t>499049033</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 밴드형 기저귀 아동공용 5단계(12kg~)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/174683688?itemId=499049033</t>
-  </si>
-  <si>
-    <t>174662956</t>
-  </si>
-  <si>
-    <t>498912308</t>
-  </si>
-  <si>
-    <t>팸퍼스 스와들러 밴드형 기저귀 6단계(16kg~)</t>
-  </si>
-  <si>
-    <t>https://www.coupang.com/vp/products/174662956?itemId=498912308</t>
-  </si>
-  <si>
-    <t>ea</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/9606247018/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=52150&amp;nvMid=9606247018&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043098&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/9606247018?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21798278124/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=51070&amp;nvMid=21798278124&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042987&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21798278124?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/20804055294/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=51600&amp;nvMid=20804055294&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042994&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/20804055294?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/20804087696/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=53760&amp;nvMid=20804087696&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043009&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/20804087696?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/24355155523/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=39040&amp;nvMid=24355155523&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043013&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=DEFAULT&amp;inflow=slc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/24355155523?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/24355221522/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=39040&amp;nvMid=24355221522&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042980&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=DEFAULT&amp;inflow=slc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/24355221522?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/24355278522/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=39040&amp;nvMid=24355278522&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043044&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=DEFAULT&amp;inflow=slc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/24355278522?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21800768787/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=49900&amp;nvMid=21800768787&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043007&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21800768787?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21800772029/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=49870&amp;nvMid=21800772029&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042987&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21800772029?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21799603401/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=40960&amp;nvMid=21799603401&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043032&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21799603401?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21799480376/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=40960&amp;nvMid=21799480376&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043053&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21799480376?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21800790512/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=41870&amp;nvMid=21800790512&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043009&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21800790512?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21793228443/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=30830&amp;nvMid=21793228443&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043002&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21793228443?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21793256416/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=29110&amp;nvMid=21793256416&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043069&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21793256416?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21793256419/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=38940&amp;nvMid=21793256419&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042980&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21793256419?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21968910906/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=30100&amp;nvMid=21968910906&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043044&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21968910906?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21793284456/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=29110&amp;nvMid=21793284456&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043052&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21793284456?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/23399582505/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=30400&amp;nvMid=23399582505&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043036&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/23399582505?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; nx_ssl=2; NID_SES=AAABmTS1qK3DWpI+vT6tS/IXepFHUqlU52hUxIURJm+79iPK1XfOsGtyEjTLKqkBk0sQr8RIBCM2l/gaS2GmNXn/UgA2MUVZ6+YYOqpStjGz1h56NZdADY8Yk00wMsACiFpi4NC9wRijk6nUifJJManEMWHfCgBl2NDaZIrclNhj5dOzd9QfarDtp9Wr8fHAv5UvTtbNg3r2EHzmpzeGTJWSRLnGdSJr24Qu4UARh4CD1Y4rs6wWpQgPK/SSzVTvyRE0DSx0kHFuvoZ7ZX4H0p3mVA71+aWu5udKNl05qDaYPJIOfr4um8UVNNe0le2Q6IHF8l5GN1mLNapVzwfsEFY8X60j7Jk+ZTZ+fM5RqBKFCoFCiKIP8P6BHSpn4971fcEcecOktT3fzttm4ICkaTEjFN9mcD6t/zQru/jVdAvBlUOKY0aX6ArdmeYhFVTwiA0aiWtlW7vhja4NkfzsvgpxIpSG+2PgvAHimvUlqOmwGGQ4Q3tTLYd0VPdob/wYqxOn0TqEomrnQ39uZ+qtItfCszRL6MAl48cOMd1NEWPdl2xR; spage_uid=' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/23684180490/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=3890&amp;nvMid=23684180490&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20042360&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.88 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/23684180490?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; NID_SES=AAABma5ukSECW7mF/lksZ2Btn/5oRoUb/jyUYQ9czyO2U9rjVNO9ePiByKaRAncKyYkHO0GSEN+us3R5PdkQq2iyUvVrLIckNc1fuqaweljaLfe9z9Y4tx+7WERcZTA9SnTiHWdYMfuo7KKnzXqtSWzdDa3IEF93Qiz27hsqcJjQurSkWYsUiVVRvUX9yMfygF9FC2f+tWfUGifJB5NgiOHIqZhQ1c1JvT1hmnhegmSXmyKeDGM+yIdxQCGF6KKNvVNd0wHqoL3qWLSkiIZhz6PZ7ZOOo2G/MBADcs0VzkLgbyzK6yQLjduY5hMdmmiPOfjrzlqc5I7ILyHa4i3ShudXv0xdsOPZJSKTamHqoeTBbY+F6csZjQzMjA7EIs9lOQKO+czwdN1op9Ak939NVLdgYhty50AT8ch9tKieq1TvLHZcqnRMtrDfrMlRgu8E/xayaNIhKtOaI7x3irXj5eh2JQbGm21tZhfXicyvdTwWVERNJy6Mpf6dBykmtHtz2JHRLWAgNdL93l4sdqQLdyWMJvSmEfCQAHXs6ymfD5QeZMkc; spage_uid=' \
-  --compressed</t>
-  </si>
 </sst>
 </file>
 
@@ -4855,13 +4841,20 @@
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5232,341 +5225,375 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="28">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="18">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="18">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="18" applyFill="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="18" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="21" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="18" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="18" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="16" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="28">
+  <cellStyles count="41">
     <cellStyle name="Accent1 2" xfId="3" xr:uid="{CD18BBF3-FE95-4D55-822D-0AA1A21D82CD}"/>
     <cellStyle name="Comma [0] 2" xfId="21" xr:uid="{A70D06FA-B7BE-4404-AA98-EBB1B9CCEF8C}"/>
     <cellStyle name="Comma 2" xfId="22" xr:uid="{9D90804A-5877-4326-AB4D-E82B030EF873}"/>
@@ -5575,26 +5602,39 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{E3027C87-3425-4354-A2E5-40D98544E226}"/>
     <cellStyle name="Normal 2 2" xfId="19" xr:uid="{C0371AF8-5E3E-4743-AC06-6C5C6725E533}"/>
+    <cellStyle name="Normal 2 2 2" xfId="39" xr:uid="{7ED4B2BE-C338-4559-8194-775925CF7492}"/>
+    <cellStyle name="Normal 2 3" xfId="28" xr:uid="{5A226FC5-7633-4ABD-A6C4-94D156567E69}"/>
     <cellStyle name="강조색1 2" xfId="11" xr:uid="{A934E348-EA5B-4334-AF0A-1E05D501C3AF}"/>
     <cellStyle name="나쁨 2" xfId="9" xr:uid="{C2AC1E40-D9C4-4553-9EC2-4A44D1F99467}"/>
     <cellStyle name="백분율 2" xfId="23" xr:uid="{FB1E9176-C109-45C2-9F73-F2F505057D68}"/>
     <cellStyle name="백분율 2 2" xfId="5" xr:uid="{02084A23-C37E-42C6-B34D-26633ADF2166}"/>
     <cellStyle name="백분율 2 2 2" xfId="14" xr:uid="{2ABD8D88-0949-47C4-931B-E229CE8EC182}"/>
+    <cellStyle name="백분율 2 2 2 2" xfId="35" xr:uid="{7CD35028-07DB-4839-97F4-F06C336BA046}"/>
+    <cellStyle name="백분율 2 2 3" xfId="30" xr:uid="{EAEB268C-78D3-4645-8979-C9DCD47C9CB7}"/>
     <cellStyle name="쉼표 [0] 2" xfId="26" xr:uid="{C97F629B-9968-46CB-897E-3FDE3E5D2787}"/>
     <cellStyle name="쉼표 [0] 2 2 10 2" xfId="13" xr:uid="{985EC853-779B-4439-BD83-87878B8C29B7}"/>
+    <cellStyle name="쉼표 [0] 2 2 10 2 2" xfId="34" xr:uid="{5758EC4D-BE1A-4423-B48E-39214134DDA6}"/>
     <cellStyle name="쉼표 [0] 3" xfId="27" xr:uid="{8E904538-A644-418B-9A4A-87051DA35DB1}"/>
     <cellStyle name="쉼표 [0] 4" xfId="25" xr:uid="{29B49EEE-F2C3-4CCE-9864-F3C86953EF41}"/>
     <cellStyle name="입력 2" xfId="10" xr:uid="{09712B67-15E2-4842-82AA-E3DCB3572D0B}"/>
     <cellStyle name="표준 12" xfId="17" xr:uid="{A379F59E-3062-4AB9-BA52-A3E4F139F891}"/>
+    <cellStyle name="표준 12 2" xfId="38" xr:uid="{D0C1F75B-0720-434C-9B2B-7AA6A1346424}"/>
     <cellStyle name="표준 2" xfId="8" xr:uid="{4AF07777-0331-4824-9328-4B8C4FA9D6B8}"/>
     <cellStyle name="표준 2 2" xfId="12" xr:uid="{2449B9C0-4AAE-4931-880D-596972103349}"/>
+    <cellStyle name="표준 2 2 2" xfId="33" xr:uid="{DE193727-13CE-4B02-B3C6-4CBD95935293}"/>
     <cellStyle name="표준 2 2 2 2" xfId="24" xr:uid="{1C16CA7A-5308-456C-A303-293AB6171C2E}"/>
     <cellStyle name="표준 2 3" xfId="7" xr:uid="{ACC88D40-2EC1-4764-AB2B-6CFC13CD2B8B}"/>
     <cellStyle name="표준 2 3 2" xfId="16" xr:uid="{51CCD5BD-0851-4347-B161-6EE92BB2C61A}"/>
+    <cellStyle name="표준 2 3 2 2" xfId="37" xr:uid="{B9F74D97-25E6-4C1F-8148-94B4F80DFC16}"/>
+    <cellStyle name="표준 2 4" xfId="32" xr:uid="{45001262-30EA-4107-AF05-2BB73A28CA74}"/>
     <cellStyle name="표준 25" xfId="20" xr:uid="{2F307373-4F3B-45D2-BF28-D41FDF6CBB89}"/>
+    <cellStyle name="표준 25 2" xfId="40" xr:uid="{5AF0BD58-7DDE-4333-B08B-4947494FAABF}"/>
     <cellStyle name="표준 3" xfId="15" xr:uid="{A157B020-D4AF-4EAE-B97C-42B65F5881CF}"/>
+    <cellStyle name="표준 3 2" xfId="36" xr:uid="{593A304E-B33F-4DD5-AE6C-5EC4203B5892}"/>
     <cellStyle name="표준 4" xfId="4" xr:uid="{99D950CB-BAA1-4230-A942-4E456B745BA6}"/>
+    <cellStyle name="표준 4 2" xfId="29" xr:uid="{C75ED153-8C33-4222-96B5-B82C02FC725D}"/>
     <cellStyle name="표준 5" xfId="6" xr:uid="{0A89C352-BF6C-489E-9EAF-1AE4462E684E}"/>
+    <cellStyle name="표준 5 2" xfId="31" xr:uid="{25D6D79A-551E-4391-8701-381D5933545C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7305,10 +7345,10 @@
   <dimension ref="A1:BJ81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="11" topLeftCell="L47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="11" topLeftCell="L44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="A50" sqref="A50:XFD50"/>
+      <selection pane="bottomRight" activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -10683,8 +10723,8 @@
       <c r="L47" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="M47" s="34" t="s">
-        <v>579</v>
+      <c r="M47" s="88" t="s">
+        <v>779</v>
       </c>
       <c r="N47" s="16">
         <v>1</v>
@@ -10769,7 +10809,7 @@
         <v>263</v>
       </c>
       <c r="M48" s="34" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="N48" s="16">
         <v>1</v>
@@ -10854,7 +10894,7 @@
         <v>267</v>
       </c>
       <c r="M49" s="34" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="N49" s="16">
         <v>1</v>
@@ -10938,9 +10978,7 @@
       <c r="L50" s="27" t="s">
         <v>453</v>
       </c>
-      <c r="M50" s="34" t="s">
-        <v>780</v>
-      </c>
+      <c r="M50" s="34"/>
       <c r="N50" s="16">
         <v>1</v>
       </c>
@@ -10948,7 +10986,7 @@
         <v>461</v>
       </c>
       <c r="P50" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q50" s="16" t="s">
         <v>418</v>
@@ -11023,7 +11061,7 @@
         <v>270</v>
       </c>
       <c r="M51" s="34" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="N51" s="16">
         <v>1</v>
@@ -11108,7 +11146,7 @@
         <v>273</v>
       </c>
       <c r="M52" s="34" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="N52" s="16">
         <v>4</v>
@@ -11192,7 +11230,7 @@
         <v>276</v>
       </c>
       <c r="M53" s="34" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="N53" s="16">
         <v>6</v>
@@ -11277,7 +11315,7 @@
         <v>278</v>
       </c>
       <c r="M54" s="34" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="N54" s="16">
         <v>6</v>
@@ -11362,7 +11400,7 @@
         <v>281</v>
       </c>
       <c r="M55" s="34" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="N55" s="16">
         <v>1</v>
@@ -11444,7 +11482,7 @@
         <v>482</v>
       </c>
       <c r="M56" s="34" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="N56" s="17">
         <v>2800</v>
@@ -11521,7 +11559,7 @@
         <v>492</v>
       </c>
       <c r="M57" s="34" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="N57" s="17">
         <v>1900</v>
@@ -11598,7 +11636,7 @@
         <v>498</v>
       </c>
       <c r="M58" s="34" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="N58" s="17">
         <v>2000</v>
@@ -11675,7 +11713,7 @@
         <v>508</v>
       </c>
       <c r="M59" s="34" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="N59" s="17">
         <v>2800</v>
@@ -11752,7 +11790,7 @@
         <v>514</v>
       </c>
       <c r="M60" s="34" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="N60" s="17">
         <v>1900</v>
@@ -11829,7 +11867,7 @@
         <v>520</v>
       </c>
       <c r="M61" s="34" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="N61" s="17">
         <v>2000</v>
@@ -11906,7 +11944,7 @@
         <v>530</v>
       </c>
       <c r="M62" s="34" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="N62" s="17">
         <v>2800</v>
@@ -11983,7 +12021,7 @@
         <v>536</v>
       </c>
       <c r="M63" s="34" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="N63" s="17">
         <v>1900</v>
@@ -12030,25 +12068,25 @@
         <v>53</v>
       </c>
       <c r="B64" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="C64" s="17" t="s">
         <v>595</v>
       </c>
-      <c r="C64" s="17" t="s">
+      <c r="D64" s="17" t="s">
         <v>596</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>597</v>
       </c>
       <c r="E64" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F64" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G64" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G64" s="17" t="s">
+      <c r="H64" s="17" t="s">
         <v>599</v>
-      </c>
-      <c r="H64" s="17" t="s">
-        <v>600</v>
       </c>
       <c r="I64" s="17">
         <v>1</v>
@@ -12057,43 +12095,43 @@
         <v>9606247018</v>
       </c>
       <c r="K64" s="17" t="s">
+        <v>652</v>
+      </c>
+      <c r="L64" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="L64" s="1" t="s">
-        <v>654</v>
-      </c>
       <c r="M64" s="71" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="N64" s="17">
         <v>184</v>
       </c>
       <c r="O64" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P64" s="17">
         <v>1</v>
       </c>
       <c r="Q64" s="17" t="s">
+        <v>688</v>
+      </c>
+      <c r="R64" s="17" t="s">
         <v>689</v>
-      </c>
-      <c r="R64" s="17" t="s">
-        <v>690</v>
       </c>
       <c r="S64" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T64" s="17" t="s">
+        <v>690</v>
+      </c>
+      <c r="U64" s="17" t="s">
         <v>691</v>
-      </c>
-      <c r="U64" s="17" t="s">
-        <v>692</v>
       </c>
       <c r="V64" s="17">
         <v>46</v>
       </c>
       <c r="W64" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X64" s="17">
         <v>4</v>
@@ -12110,25 +12148,25 @@
         <v>54</v>
       </c>
       <c r="B65" s="17" t="s">
+        <v>600</v>
+      </c>
+      <c r="C65" s="17" t="s">
         <v>601</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="D65" s="17" t="s">
         <v>602</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>603</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F65" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G65" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G65" s="17" t="s">
+      <c r="H65" s="17" t="s">
         <v>599</v>
-      </c>
-      <c r="H65" s="17" t="s">
-        <v>600</v>
       </c>
       <c r="I65" s="17">
         <v>2</v>
@@ -12137,43 +12175,43 @@
         <v>21798278124</v>
       </c>
       <c r="K65" s="17" t="s">
+        <v>654</v>
+      </c>
+      <c r="L65" s="1" t="s">
         <v>655</v>
       </c>
-      <c r="L65" s="1" t="s">
-        <v>656</v>
-      </c>
       <c r="M65" s="71" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="N65" s="17">
         <v>168</v>
       </c>
       <c r="O65" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P65" s="17">
         <v>1</v>
       </c>
       <c r="Q65" s="17" t="s">
+        <v>692</v>
+      </c>
+      <c r="R65" s="17" t="s">
         <v>693</v>
-      </c>
-      <c r="R65" s="17" t="s">
-        <v>694</v>
       </c>
       <c r="S65" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T65" s="17" t="s">
+        <v>694</v>
+      </c>
+      <c r="U65" s="17" t="s">
         <v>695</v>
-      </c>
-      <c r="U65" s="17" t="s">
-        <v>696</v>
       </c>
       <c r="V65" s="17">
         <v>42</v>
       </c>
       <c r="W65" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X65" s="17">
         <v>4</v>
@@ -12190,25 +12228,25 @@
         <v>55</v>
       </c>
       <c r="B66" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="C66" s="17" t="s">
         <v>604</v>
       </c>
-      <c r="C66" s="17" t="s">
+      <c r="D66" s="17" t="s">
         <v>605</v>
-      </c>
-      <c r="D66" s="17" t="s">
-        <v>606</v>
       </c>
       <c r="E66" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F66" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G66" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G66" s="17" t="s">
+      <c r="H66" s="17" t="s">
         <v>599</v>
-      </c>
-      <c r="H66" s="17" t="s">
-        <v>600</v>
       </c>
       <c r="I66" s="17">
         <v>3</v>
@@ -12217,43 +12255,43 @@
         <v>20804055294</v>
       </c>
       <c r="K66" s="17" t="s">
+        <v>656</v>
+      </c>
+      <c r="L66" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="L66" s="1" t="s">
-        <v>658</v>
-      </c>
       <c r="M66" s="71" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="N66" s="17">
         <v>144</v>
       </c>
       <c r="O66" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P66" s="17">
         <v>1</v>
       </c>
       <c r="Q66" s="17" t="s">
+        <v>696</v>
+      </c>
+      <c r="R66" s="17" t="s">
         <v>697</v>
-      </c>
-      <c r="R66" s="17" t="s">
-        <v>698</v>
       </c>
       <c r="S66" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T66" s="17" t="s">
+        <v>698</v>
+      </c>
+      <c r="U66" s="17" t="s">
         <v>699</v>
-      </c>
-      <c r="U66" s="17" t="s">
-        <v>700</v>
       </c>
       <c r="V66" s="17">
         <v>36</v>
       </c>
       <c r="W66" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X66" s="17">
         <v>4</v>
@@ -12270,25 +12308,25 @@
         <v>56</v>
       </c>
       <c r="B67" s="17" t="s">
+        <v>606</v>
+      </c>
+      <c r="C67" s="17" t="s">
         <v>607</v>
       </c>
-      <c r="C67" s="17" t="s">
+      <c r="D67" s="17" t="s">
         <v>608</v>
-      </c>
-      <c r="D67" s="17" t="s">
-        <v>609</v>
       </c>
       <c r="E67" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F67" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G67" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G67" s="17" t="s">
+      <c r="H67" s="17" t="s">
         <v>599</v>
-      </c>
-      <c r="H67" s="17" t="s">
-        <v>600</v>
       </c>
       <c r="I67" s="17">
         <v>4</v>
@@ -12297,43 +12335,43 @@
         <v>20804087696</v>
       </c>
       <c r="K67" s="17" t="s">
+        <v>658</v>
+      </c>
+      <c r="L67" s="1" t="s">
         <v>659</v>
       </c>
-      <c r="L67" s="1" t="s">
-        <v>660</v>
-      </c>
       <c r="M67" s="71" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="N67" s="17">
         <v>112</v>
       </c>
       <c r="O67" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P67" s="17">
         <v>1</v>
       </c>
       <c r="Q67" s="17" t="s">
+        <v>700</v>
+      </c>
+      <c r="R67" s="17" t="s">
         <v>701</v>
-      </c>
-      <c r="R67" s="17" t="s">
-        <v>702</v>
       </c>
       <c r="S67" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T67" s="17" t="s">
+        <v>702</v>
+      </c>
+      <c r="U67" s="17" t="s">
         <v>703</v>
-      </c>
-      <c r="U67" s="17" t="s">
-        <v>704</v>
       </c>
       <c r="V67" s="17">
         <v>28</v>
       </c>
       <c r="W67" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X67" s="17">
         <v>4</v>
@@ -12350,25 +12388,25 @@
         <v>57</v>
       </c>
       <c r="B68" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="C68" s="17" t="s">
         <v>610</v>
       </c>
-      <c r="C68" s="17" t="s">
+      <c r="D68" s="17" t="s">
         <v>611</v>
-      </c>
-      <c r="D68" s="17" t="s">
-        <v>612</v>
       </c>
       <c r="E68" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F68" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G68" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G68" s="17" t="s">
+      <c r="H68" s="17" t="s">
         <v>599</v>
-      </c>
-      <c r="H68" s="17" t="s">
-        <v>600</v>
       </c>
       <c r="I68" s="17">
         <v>5</v>
@@ -12377,43 +12415,43 @@
         <v>24355155523</v>
       </c>
       <c r="K68" s="17" t="s">
+        <v>660</v>
+      </c>
+      <c r="L68" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="L68" s="1" t="s">
-        <v>662</v>
-      </c>
       <c r="M68" s="71" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="N68" s="17">
         <v>120</v>
       </c>
       <c r="O68" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P68" s="17">
         <v>1</v>
       </c>
       <c r="Q68" s="17" t="s">
+        <v>704</v>
+      </c>
+      <c r="R68" s="17" t="s">
         <v>705</v>
-      </c>
-      <c r="R68" s="17" t="s">
-        <v>706</v>
       </c>
       <c r="S68" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T68" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="U68" s="17" t="s">
         <v>707</v>
-      </c>
-      <c r="U68" s="17" t="s">
-        <v>708</v>
       </c>
       <c r="V68" s="17">
         <v>30</v>
       </c>
       <c r="W68" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X68" s="17">
         <v>4</v>
@@ -12430,25 +12468,25 @@
         <v>58</v>
       </c>
       <c r="B69" s="17" t="s">
+        <v>612</v>
+      </c>
+      <c r="C69" s="17" t="s">
         <v>613</v>
       </c>
-      <c r="C69" s="17" t="s">
+      <c r="D69" s="17" t="s">
         <v>614</v>
-      </c>
-      <c r="D69" s="17" t="s">
-        <v>615</v>
       </c>
       <c r="E69" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F69" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G69" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G69" s="17" t="s">
+      <c r="H69" s="17" t="s">
         <v>599</v>
-      </c>
-      <c r="H69" s="17" t="s">
-        <v>600</v>
       </c>
       <c r="I69" s="17">
         <v>6</v>
@@ -12457,43 +12495,43 @@
         <v>24355221522</v>
       </c>
       <c r="K69" s="17" t="s">
+        <v>662</v>
+      </c>
+      <c r="L69" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="L69" s="1" t="s">
-        <v>664</v>
-      </c>
       <c r="M69" s="71" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="N69" s="17">
         <v>104</v>
       </c>
       <c r="O69" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P69" s="17">
         <v>1</v>
       </c>
       <c r="Q69" s="17" t="s">
+        <v>708</v>
+      </c>
+      <c r="R69" s="17" t="s">
         <v>709</v>
-      </c>
-      <c r="R69" s="17" t="s">
-        <v>710</v>
       </c>
       <c r="S69" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T69" s="17" t="s">
+        <v>710</v>
+      </c>
+      <c r="U69" s="17" t="s">
         <v>711</v>
-      </c>
-      <c r="U69" s="17" t="s">
-        <v>712</v>
       </c>
       <c r="V69" s="17">
         <v>26</v>
       </c>
       <c r="W69" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X69" s="17">
         <v>4</v>
@@ -12510,25 +12548,25 @@
         <v>59</v>
       </c>
       <c r="B70" s="17" t="s">
+        <v>615</v>
+      </c>
+      <c r="C70" s="17" t="s">
         <v>616</v>
       </c>
-      <c r="C70" s="17" t="s">
+      <c r="D70" s="17" t="s">
         <v>617</v>
-      </c>
-      <c r="D70" s="17" t="s">
-        <v>618</v>
       </c>
       <c r="E70" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F70" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G70" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G70" s="17" t="s">
+      <c r="H70" s="17" t="s">
         <v>599</v>
-      </c>
-      <c r="H70" s="17" t="s">
-        <v>600</v>
       </c>
       <c r="I70" s="17">
         <v>7</v>
@@ -12537,43 +12575,43 @@
         <v>24355278522</v>
       </c>
       <c r="K70" s="17" t="s">
+        <v>664</v>
+      </c>
+      <c r="L70" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="L70" s="1" t="s">
-        <v>666</v>
-      </c>
       <c r="M70" s="71" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="N70" s="17">
         <v>88</v>
       </c>
       <c r="O70" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P70" s="17">
         <v>1</v>
       </c>
       <c r="Q70" s="17" t="s">
+        <v>712</v>
+      </c>
+      <c r="R70" s="17" t="s">
         <v>713</v>
-      </c>
-      <c r="R70" s="17" t="s">
-        <v>714</v>
       </c>
       <c r="S70" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T70" s="17" t="s">
+        <v>714</v>
+      </c>
+      <c r="U70" s="17" t="s">
         <v>715</v>
-      </c>
-      <c r="U70" s="17" t="s">
-        <v>716</v>
       </c>
       <c r="V70" s="17">
         <v>22</v>
       </c>
       <c r="W70" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X70" s="17">
         <v>4</v>
@@ -12590,25 +12628,25 @@
         <v>60</v>
       </c>
       <c r="B71" s="17" t="s">
+        <v>618</v>
+      </c>
+      <c r="C71" s="17" t="s">
         <v>619</v>
       </c>
-      <c r="C71" s="17" t="s">
+      <c r="D71" s="17" t="s">
         <v>620</v>
-      </c>
-      <c r="D71" s="17" t="s">
-        <v>621</v>
       </c>
       <c r="E71" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F71" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G71" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G71" s="17" t="s">
-        <v>599</v>
-      </c>
       <c r="H71" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I71" s="17">
         <v>8</v>
@@ -12617,43 +12655,43 @@
         <v>21800768787</v>
       </c>
       <c r="K71" s="17" t="s">
+        <v>666</v>
+      </c>
+      <c r="L71" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="L71" s="1" t="s">
-        <v>668</v>
-      </c>
       <c r="M71" s="71" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="N71" s="17">
         <v>186</v>
       </c>
       <c r="O71" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P71" s="17">
         <v>1</v>
       </c>
       <c r="Q71" s="17" t="s">
+        <v>716</v>
+      </c>
+      <c r="R71" s="17" t="s">
         <v>717</v>
-      </c>
-      <c r="R71" s="17" t="s">
-        <v>718</v>
       </c>
       <c r="S71" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T71" s="17" t="s">
+        <v>718</v>
+      </c>
+      <c r="U71" s="17" t="s">
         <v>719</v>
-      </c>
-      <c r="U71" s="17" t="s">
-        <v>720</v>
       </c>
       <c r="V71" s="17">
         <v>186</v>
       </c>
       <c r="W71" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X71" s="17">
         <v>1</v>
@@ -12670,25 +12708,25 @@
         <v>61</v>
       </c>
       <c r="B72" s="17" t="s">
+        <v>622</v>
+      </c>
+      <c r="C72" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="C72" s="17" t="s">
+      <c r="D72" s="17" t="s">
         <v>624</v>
-      </c>
-      <c r="D72" s="17" t="s">
-        <v>625</v>
       </c>
       <c r="E72" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F72" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G72" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G72" s="17" t="s">
-        <v>599</v>
-      </c>
       <c r="H72" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I72" s="17">
         <v>9</v>
@@ -12697,43 +12735,43 @@
         <v>21800772029</v>
       </c>
       <c r="K72" s="17" t="s">
+        <v>668</v>
+      </c>
+      <c r="L72" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="L72" s="1" t="s">
-        <v>670</v>
-      </c>
       <c r="M72" s="71" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="N72" s="17">
         <v>168</v>
       </c>
       <c r="O72" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P72" s="17">
         <v>1</v>
       </c>
       <c r="Q72" s="17" t="s">
+        <v>720</v>
+      </c>
+      <c r="R72" s="17" t="s">
         <v>721</v>
-      </c>
-      <c r="R72" s="17" t="s">
-        <v>722</v>
       </c>
       <c r="S72" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T72" s="17" t="s">
+        <v>722</v>
+      </c>
+      <c r="U72" s="17" t="s">
         <v>723</v>
-      </c>
-      <c r="U72" s="17" t="s">
-        <v>724</v>
       </c>
       <c r="V72" s="17">
         <v>168</v>
       </c>
       <c r="W72" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X72" s="17">
         <v>1</v>
@@ -12750,25 +12788,25 @@
         <v>62</v>
       </c>
       <c r="B73" s="17" t="s">
+        <v>625</v>
+      </c>
+      <c r="C73" s="17" t="s">
         <v>626</v>
       </c>
-      <c r="C73" s="17" t="s">
+      <c r="D73" s="17" t="s">
         <v>627</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>628</v>
       </c>
       <c r="E73" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F73" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G73" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G73" s="17" t="s">
-        <v>599</v>
-      </c>
       <c r="H73" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I73" s="17">
         <v>10</v>
@@ -12777,43 +12815,43 @@
         <v>21799603401</v>
       </c>
       <c r="K73" s="17" t="s">
+        <v>670</v>
+      </c>
+      <c r="L73" s="1" t="s">
         <v>671</v>
       </c>
-      <c r="L73" s="1" t="s">
-        <v>672</v>
-      </c>
       <c r="M73" s="71" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="N73" s="17">
         <v>150</v>
       </c>
       <c r="O73" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P73" s="17">
         <v>1</v>
       </c>
       <c r="Q73" s="17" t="s">
+        <v>724</v>
+      </c>
+      <c r="R73" s="17" t="s">
         <v>725</v>
-      </c>
-      <c r="R73" s="17" t="s">
-        <v>726</v>
       </c>
       <c r="S73" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T73" s="17" t="s">
+        <v>726</v>
+      </c>
+      <c r="U73" s="17" t="s">
         <v>727</v>
-      </c>
-      <c r="U73" s="17" t="s">
-        <v>728</v>
       </c>
       <c r="V73" s="17">
         <v>150</v>
       </c>
       <c r="W73" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X73" s="17">
         <v>1</v>
@@ -12830,25 +12868,25 @@
         <v>63</v>
       </c>
       <c r="B74" s="17" t="s">
+        <v>628</v>
+      </c>
+      <c r="C74" s="17" t="s">
         <v>629</v>
       </c>
-      <c r="C74" s="17" t="s">
+      <c r="D74" s="17" t="s">
         <v>630</v>
-      </c>
-      <c r="D74" s="17" t="s">
-        <v>631</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F74" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G74" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G74" s="17" t="s">
-        <v>599</v>
-      </c>
       <c r="H74" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I74" s="17">
         <v>11</v>
@@ -12857,43 +12895,43 @@
         <v>21799480376</v>
       </c>
       <c r="K74" s="17" t="s">
+        <v>672</v>
+      </c>
+      <c r="L74" s="1" t="s">
         <v>673</v>
       </c>
-      <c r="L74" s="1" t="s">
-        <v>674</v>
-      </c>
       <c r="M74" s="71" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="N74" s="17">
         <v>132</v>
       </c>
       <c r="O74" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P74" s="17">
         <v>1</v>
       </c>
       <c r="Q74" s="17" t="s">
+        <v>728</v>
+      </c>
+      <c r="R74" s="17" t="s">
         <v>729</v>
-      </c>
-      <c r="R74" s="17" t="s">
-        <v>730</v>
       </c>
       <c r="S74" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T74" s="17" t="s">
+        <v>730</v>
+      </c>
+      <c r="U74" s="17" t="s">
         <v>731</v>
-      </c>
-      <c r="U74" s="17" t="s">
-        <v>732</v>
       </c>
       <c r="V74" s="17">
         <v>132</v>
       </c>
       <c r="W74" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X74" s="17">
         <v>1</v>
@@ -12910,25 +12948,25 @@
         <v>64</v>
       </c>
       <c r="B75" s="17" t="s">
+        <v>631</v>
+      </c>
+      <c r="C75" s="17" t="s">
         <v>632</v>
       </c>
-      <c r="C75" s="17" t="s">
+      <c r="D75" s="17" t="s">
         <v>633</v>
-      </c>
-      <c r="D75" s="17" t="s">
-        <v>634</v>
       </c>
       <c r="E75" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F75" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G75" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G75" s="17" t="s">
-        <v>599</v>
-      </c>
       <c r="H75" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I75" s="17">
         <v>12</v>
@@ -12937,43 +12975,43 @@
         <v>21800790512</v>
       </c>
       <c r="K75" s="17" t="s">
+        <v>674</v>
+      </c>
+      <c r="L75" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="L75" s="1" t="s">
-        <v>676</v>
-      </c>
       <c r="M75" s="71" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="N75" s="17">
         <v>112</v>
       </c>
       <c r="O75" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P75" s="17">
         <v>1</v>
       </c>
       <c r="Q75" s="17" t="s">
+        <v>732</v>
+      </c>
+      <c r="R75" s="17" t="s">
         <v>733</v>
-      </c>
-      <c r="R75" s="17" t="s">
-        <v>734</v>
       </c>
       <c r="S75" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T75" s="17" t="s">
+        <v>734</v>
+      </c>
+      <c r="U75" s="17" t="s">
         <v>735</v>
-      </c>
-      <c r="U75" s="17" t="s">
-        <v>736</v>
       </c>
       <c r="V75" s="17">
         <v>112</v>
       </c>
       <c r="W75" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X75" s="17">
         <v>1</v>
@@ -12990,25 +13028,25 @@
         <v>65</v>
       </c>
       <c r="B76" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="C76" s="17" t="s">
         <v>635</v>
       </c>
-      <c r="C76" s="17" t="s">
+      <c r="D76" s="17" t="s">
         <v>636</v>
-      </c>
-      <c r="D76" s="17" t="s">
-        <v>637</v>
       </c>
       <c r="E76" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F76" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G76" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G76" s="17" t="s">
-        <v>599</v>
-      </c>
       <c r="H76" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I76" s="17">
         <v>13</v>
@@ -13017,43 +13055,43 @@
         <v>21793228443</v>
       </c>
       <c r="K76" s="17" t="s">
+        <v>676</v>
+      </c>
+      <c r="L76" s="1" t="s">
         <v>677</v>
       </c>
-      <c r="L76" s="1" t="s">
-        <v>678</v>
-      </c>
       <c r="M76" s="71" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="N76" s="17">
         <v>128</v>
       </c>
       <c r="O76" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P76" s="17">
         <v>1</v>
       </c>
       <c r="Q76" s="17" t="s">
+        <v>736</v>
+      </c>
+      <c r="R76" s="17" t="s">
         <v>737</v>
-      </c>
-      <c r="R76" s="17" t="s">
-        <v>738</v>
       </c>
       <c r="S76" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T76" s="17" t="s">
+        <v>738</v>
+      </c>
+      <c r="U76" s="17" t="s">
         <v>739</v>
-      </c>
-      <c r="U76" s="17" t="s">
-        <v>740</v>
       </c>
       <c r="V76" s="17">
         <v>32</v>
       </c>
       <c r="W76" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X76" s="17">
         <v>4</v>
@@ -13070,25 +13108,25 @@
         <v>66</v>
       </c>
       <c r="B77" s="17" t="s">
+        <v>637</v>
+      </c>
+      <c r="C77" s="17" t="s">
         <v>638</v>
       </c>
-      <c r="C77" s="17" t="s">
+      <c r="D77" s="17" t="s">
         <v>639</v>
-      </c>
-      <c r="D77" s="17" t="s">
-        <v>640</v>
       </c>
       <c r="E77" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F77" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G77" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G77" s="17" t="s">
-        <v>599</v>
-      </c>
       <c r="H77" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I77" s="17">
         <v>14</v>
@@ -13097,43 +13135,43 @@
         <v>21793256416</v>
       </c>
       <c r="K77" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="L77" s="1" t="s">
         <v>679</v>
       </c>
-      <c r="L77" s="1" t="s">
-        <v>680</v>
-      </c>
       <c r="M77" s="71" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="N77" s="17">
         <v>116</v>
       </c>
       <c r="O77" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P77" s="17">
         <v>1</v>
       </c>
       <c r="Q77" s="17" t="s">
+        <v>740</v>
+      </c>
+      <c r="R77" s="17" t="s">
         <v>741</v>
-      </c>
-      <c r="R77" s="17" t="s">
-        <v>742</v>
       </c>
       <c r="S77" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T77" s="17" t="s">
+        <v>742</v>
+      </c>
+      <c r="U77" s="17" t="s">
         <v>743</v>
-      </c>
-      <c r="U77" s="17" t="s">
-        <v>744</v>
       </c>
       <c r="V77" s="17">
         <v>29</v>
       </c>
       <c r="W77" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X77" s="17">
         <v>4</v>
@@ -13150,25 +13188,25 @@
         <v>67</v>
       </c>
       <c r="B78" s="17" t="s">
+        <v>640</v>
+      </c>
+      <c r="C78" s="17" t="s">
         <v>641</v>
       </c>
-      <c r="C78" s="17" t="s">
+      <c r="D78" s="17" t="s">
         <v>642</v>
-      </c>
-      <c r="D78" s="17" t="s">
-        <v>643</v>
       </c>
       <c r="E78" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F78" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G78" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G78" s="17" t="s">
-        <v>599</v>
-      </c>
       <c r="H78" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I78" s="17">
         <v>15</v>
@@ -13177,43 +13215,43 @@
         <v>21793256419</v>
       </c>
       <c r="K78" s="17" t="s">
+        <v>680</v>
+      </c>
+      <c r="L78" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="L78" s="1" t="s">
-        <v>682</v>
-      </c>
       <c r="M78" s="71" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="N78" s="17">
         <v>104</v>
       </c>
       <c r="O78" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P78" s="17">
         <v>1</v>
       </c>
       <c r="Q78" s="17" t="s">
+        <v>744</v>
+      </c>
+      <c r="R78" s="17" t="s">
         <v>745</v>
-      </c>
-      <c r="R78" s="17" t="s">
-        <v>746</v>
       </c>
       <c r="S78" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T78" s="17" t="s">
+        <v>746</v>
+      </c>
+      <c r="U78" s="17" t="s">
         <v>747</v>
-      </c>
-      <c r="U78" s="17" t="s">
-        <v>748</v>
       </c>
       <c r="V78" s="17">
         <v>26</v>
       </c>
       <c r="W78" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X78" s="17">
         <v>4</v>
@@ -13230,25 +13268,25 @@
         <v>68</v>
       </c>
       <c r="B79" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="C79" s="17" t="s">
         <v>644</v>
       </c>
-      <c r="C79" s="17" t="s">
+      <c r="D79" s="17" t="s">
         <v>645</v>
-      </c>
-      <c r="D79" s="17" t="s">
-        <v>646</v>
       </c>
       <c r="E79" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F79" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G79" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G79" s="17" t="s">
-        <v>599</v>
-      </c>
       <c r="H79" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I79" s="17">
         <v>16</v>
@@ -13257,43 +13295,43 @@
         <v>21968910906</v>
       </c>
       <c r="K79" s="17" t="s">
+        <v>682</v>
+      </c>
+      <c r="L79" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="L79" s="1" t="s">
-        <v>684</v>
-      </c>
       <c r="M79" s="71" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="N79" s="17">
         <v>88</v>
       </c>
       <c r="O79" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P79" s="17">
         <v>1</v>
       </c>
       <c r="Q79" s="17" t="s">
+        <v>748</v>
+      </c>
+      <c r="R79" s="17" t="s">
         <v>749</v>
-      </c>
-      <c r="R79" s="17" t="s">
-        <v>750</v>
       </c>
       <c r="S79" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T79" s="17" t="s">
+        <v>750</v>
+      </c>
+      <c r="U79" s="17" t="s">
         <v>751</v>
-      </c>
-      <c r="U79" s="17" t="s">
-        <v>752</v>
       </c>
       <c r="V79" s="17">
         <v>22</v>
       </c>
       <c r="W79" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X79" s="17">
         <v>4</v>
@@ -13310,25 +13348,25 @@
         <v>69</v>
       </c>
       <c r="B80" s="17" t="s">
+        <v>646</v>
+      </c>
+      <c r="C80" s="17" t="s">
         <v>647</v>
       </c>
-      <c r="C80" s="17" t="s">
+      <c r="D80" s="17" t="s">
         <v>648</v>
-      </c>
-      <c r="D80" s="17" t="s">
-        <v>649</v>
       </c>
       <c r="E80" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F80" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G80" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G80" s="17" t="s">
-        <v>599</v>
-      </c>
       <c r="H80" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I80" s="17">
         <v>17</v>
@@ -13337,43 +13375,43 @@
         <v>21793284456</v>
       </c>
       <c r="K80" s="17" t="s">
+        <v>684</v>
+      </c>
+      <c r="L80" s="1" t="s">
         <v>685</v>
       </c>
-      <c r="L80" s="1" t="s">
-        <v>686</v>
-      </c>
       <c r="M80" s="71" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="N80" s="17">
         <v>76</v>
       </c>
       <c r="O80" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P80" s="17">
         <v>1</v>
       </c>
       <c r="Q80" s="17" t="s">
+        <v>752</v>
+      </c>
+      <c r="R80" s="17" t="s">
         <v>753</v>
-      </c>
-      <c r="R80" s="17" t="s">
-        <v>754</v>
       </c>
       <c r="S80" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T80" s="17" t="s">
+        <v>754</v>
+      </c>
+      <c r="U80" s="17" t="s">
         <v>755</v>
-      </c>
-      <c r="U80" s="17" t="s">
-        <v>756</v>
       </c>
       <c r="V80" s="17">
         <v>19</v>
       </c>
       <c r="W80" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X80" s="17">
         <v>4</v>
@@ -13390,25 +13428,25 @@
         <v>70</v>
       </c>
       <c r="B81" s="17" t="s">
+        <v>649</v>
+      </c>
+      <c r="C81" s="17" t="s">
         <v>650</v>
       </c>
-      <c r="C81" s="17" t="s">
+      <c r="D81" s="17" t="s">
         <v>651</v>
-      </c>
-      <c r="D81" s="17" t="s">
-        <v>652</v>
       </c>
       <c r="E81" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F81" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G81" s="17" t="s">
         <v>598</v>
       </c>
-      <c r="G81" s="17" t="s">
-        <v>599</v>
-      </c>
       <c r="H81" s="17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I81" s="17">
         <v>18</v>
@@ -13417,43 +13455,43 @@
         <v>23399582505</v>
       </c>
       <c r="K81" s="17" t="s">
+        <v>686</v>
+      </c>
+      <c r="L81" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="L81" s="1" t="s">
-        <v>688</v>
-      </c>
       <c r="M81" s="71" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="N81" s="17">
         <v>64</v>
       </c>
       <c r="O81" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="P81" s="17">
         <v>1</v>
       </c>
       <c r="Q81" s="17" t="s">
+        <v>756</v>
+      </c>
+      <c r="R81" s="17" t="s">
         <v>757</v>
-      </c>
-      <c r="R81" s="17" t="s">
-        <v>758</v>
       </c>
       <c r="S81" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T81" s="17" t="s">
+        <v>758</v>
+      </c>
+      <c r="U81" s="17" t="s">
         <v>759</v>
-      </c>
-      <c r="U81" s="17" t="s">
-        <v>760</v>
       </c>
       <c r="V81" s="17">
         <v>16</v>
       </c>
       <c r="W81" s="17" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="X81" s="17">
         <v>4</v>
@@ -13482,7 +13520,7 @@
     <mergeCell ref="AF10:AK10"/>
     <mergeCell ref="AL10:AR10"/>
   </mergeCells>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <hyperlinks>
     <hyperlink ref="L12" r:id="rId1" xr:uid="{02F06F4D-B718-44A4-B9E3-F729BA20DD3D}"/>
     <hyperlink ref="U13" r:id="rId2" display="https://www.coupang.com/vp/products/8403247?itemId=1038077450" xr:uid="{7C1FF7DE-3286-4824-918F-F17782633E5A}"/>
@@ -17662,7 +17700,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <hyperlinks>
     <hyperlink ref="L34" r:id="rId1" xr:uid="{7D72E9DA-EC00-4F34-B30D-0005603F18B2}"/>
     <hyperlink ref="L40" r:id="rId2" xr:uid="{06662602-3C7D-4485-A282-D19EF8A00FF6}"/>
@@ -17789,7 +17827,7 @@
       <c r="C3" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -17816,7 +17854,7 @@
       <c r="A2" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -17885,28 +17923,13 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100764EA4CBCC3EB840B3A71EC084A37A79" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1c63f6b0f6065541758bb15ee54f6821">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9ed8ad31-4880-4d63-8f72-0ebd22f8068c" xmlns:ns4="819a0a68-6060-4071-a88e-471cccc4a5a4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0011b285b55bc13472d229a8f23f1c52" ns3:_="" ns4:_="">
     <xsd:import namespace="9ed8ad31-4880-4d63-8f72-0ebd22f8068c"/>
@@ -18123,7 +18146,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6D1DAC1-61BB-432E-B17D-AB35AE99FFBA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9ed8ad31-4880-4d63-8f72-0ebd22f8068c"/>
+    <ds:schemaRef ds:uri="819a0a68-6060-4071-a88e-471cccc4a5a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{538AE23B-FCFE-430C-92AD-3D09EEFD4655}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -18140,29 +18197,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAA63007-5F77-494C-AF11-EF28F74AE67F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6D1DAC1-61BB-432E-B17D-AB35AE99FFBA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9ed8ad31-4880-4d63-8f72-0ebd22f8068c"/>
-    <ds:schemaRef ds:uri="819a0a68-6060-4071-a88e-471cccc4a5a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
CURL Information update & disable chrome driver
</commit_message>
<xml_diff>
--- a/data/Liberation_Price Tracker SKU list_v1_Pampers.xlsx
+++ b/data/Liberation_Price Tracker SKU list_v1_Pampers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kang.y.5\OneDrive - Procter and Gamble\Documents\GitHub\liberation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pgone-my.sharepoint.com/personal/kang_y_5_pg_com1/Documents/Documents/GitHub/liberation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{17BCC08E-1F5D-4046-8FCF-30AF4568CA99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{877B6FAB-9E00-409C-AAB5-780CC33C6F76}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{17BCC08E-1F5D-4046-8FCF-30AF4568CA99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{52AFDCC4-1218-4CBF-BD7A-C59473120D2A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="779" xr2:uid="{082D8A25-05B0-4134-80F4-C81249D6F8B7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="784">
   <si>
     <t>No</t>
     <phoneticPr fontId="5"/>
@@ -3630,20 +3630,6 @@
   --compressed</t>
   </si>
   <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/6999016004/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=13040&amp;nvMid=6999016004&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013178&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/6999016004?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ncpa=692492|kh44ogk0|9fb3b998758574bea83060c00d5f6a728db3a7a5|s_a072289e9d4f|083814cd5b605d5608ff74b7f09f6f68184ca97f:221844|kh44u848|395aa407aa9c951d73d8de3fa3ce656c5d6ef428|s_1a7f4dd73489|97a684e827d8975db0e10abff1118b51d7a85ffa:1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:845657|kh45wqow|5cad2ef28fafd769103a495fa86c4510ccd30c82|s_54853016347d|9e6dc8c0e97a9ab511f0b55a0ba1cd5db2522760:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:24|kh46h9w0|514e6e49616c349dc94d31b9a85cd9a43485113d|s_419afe53a6bb|1f0c44bb64e6ca64f62753fde0a6e9a30d925da0:17703|kh5yj708|1b94217d27ff92d18e091e4b26be526631f2b666|s_1f0b6dd345b2|8da79206b3c0d93283e34b5f8e2e5540b8a420ff:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077' \
-  --compressed</t>
-  </si>
-  <si>
     <t>curl 'https://search.shopping.naver.com/catalog/22470992398/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=13300&amp;nvMid=22470992398&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013178&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=DEFAULT&amp;inflow=slc' \
   -H 'Connection: keep-alive' \
   -H 'Accept: application/json, text/plain, */*' \
@@ -3728,34 +3714,6 @@
   --compressed</t>
   </si>
   <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/9803321078/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=26020&amp;nvMid=9803321078&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20040510&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/9803321078?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ncpa=692492|kh44ogk0|9fb3b998758574bea83060c00d5f6a728db3a7a5|s_a072289e9d4f|083814cd5b605d5608ff74b7f09f6f68184ca97f:221844|kh44u848|395aa407aa9c951d73d8de3fa3ce656c5d6ef428|s_1a7f4dd73489|97a684e827d8975db0e10abff1118b51d7a85ffa:1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:845657|kh45wqow|5cad2ef28fafd769103a495fa86c4510ccd30c82|s_54853016347d|9e6dc8c0e97a9ab511f0b55a0ba1cd5db2522760:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:24|kh46h9w0|514e6e49616c349dc94d31b9a85cd9a43485113d|s_419afe53a6bb|1f0c44bb64e6ca64f62753fde0a6e9a30d925da0:17703|kh5yj708|1b94217d27ff92d18e091e4b26be526631f2b666|s_1f0b6dd345b2|8da79206b3c0d93283e34b5f8e2e5540b8a420ff:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077' \
-  --compressed</t>
-  </si>
-  <si>
-    <t>curl 'https://search.shopping.naver.com/catalog/21151605555/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=15900&amp;nvMid=21151605555&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20040506&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
-  -H 'Connection: keep-alive' \
-  -H 'Accept: application/json, text/plain, */*' \
-  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.183 Safari/537.36' \
-  -H 'urlprefix: /api' \
-  -H 'Sec-Fetch-Site: same-origin' \
-  -H 'Sec-Fetch-Mode: cors' \
-  -H 'Sec-Fetch-Dest: empty' \
-  -H 'Referer: https://search.shopping.naver.com/catalog/21151605555?' \
-  -H 'Accept-Language: en-US,en;q=0.9' \
-  -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ncpa=692492|kh44ogk0|9fb3b998758574bea83060c00d5f6a728db3a7a5|s_a072289e9d4f|083814cd5b605d5608ff74b7f09f6f68184ca97f:221844|kh44u848|395aa407aa9c951d73d8de3fa3ce656c5d6ef428|s_1a7f4dd73489|97a684e827d8975db0e10abff1118b51d7a85ffa:1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:845657|kh45wqow|5cad2ef28fafd769103a495fa86c4510ccd30c82|s_54853016347d|9e6dc8c0e97a9ab511f0b55a0ba1cd5db2522760:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:24|kh46h9w0|514e6e49616c349dc94d31b9a85cd9a43485113d|s_419afe53a6bb|1f0c44bb64e6ca64f62753fde0a6e9a30d925da0:17703|kh5yj708|1b94217d27ff92d18e091e4b26be526631f2b666|s_1f0b6dd345b2|8da79206b3c0d93283e34b5f8e2e5540b8a420ff:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077' \
-  --compressed</t>
-  </si>
-  <si>
     <t>curl 'https://search.shopping.naver.com/catalog/12957053771/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=8900&amp;nvMid=12957053771&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20043744&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
   -H 'Connection: keep-alive' \
   -H 'Accept: application/json, text/plain, */*' \
@@ -4828,6 +4786,104 @@
   -H 'Referer: https://search.shopping.naver.com/catalog/9768921714?' \
   -H 'Accept-Language: en-US,en;q=0.9' \
   -H 'Cookie: NRTK=ag#all_gr#1_ma#-2_si#0_en#0_sp#0; NNB=YRI2QKEH7ZPV6; AD_SHP_BID=20; _fbp=fb.1.1600237181251.1334484357; ASID=a5e16e78000001749a4b44720000004f; JSESSIONID=B97147D123A3BAE0BA02B1F1DC7EDC3A; nx_ssl=2; nid_inf=846535377; NID_JKL=vwZeHz2Ai+/KobLyY80BAoa3AxIDqnfSnG6LKXroCvk=; _gid=GA1.2.987341160.1604886398; _sm_au_c=kvugCACWrBNtImttRtInEgt0Z9xIe8wh0TSgmu+4MVdwgAAAAEW2S4sXIJj9DhEinawHv8QG9V8wR4TPurbGznW09G3I=; ssm_au_c=kvugCAI42qychAgQgY3v7aq/4gIPAzbmgJXaveXORwwUgAAAAcPcgMW/ef1oFc2tihcgIgboaNDwfpr2zgeJglHLC/dE=; BMR=s=1605062626641&amp;r=https%3A%2F%2Fm.blog.naver.com%2FPostView.nhn%3FblogId%3Dflowerringg%26logNo%3D221346922190%26proxyReferer%3Dhttps%3A%252F%252Fwww.google.com%252F&amp;r2=https%3A%2F%2Fwww.google.com%2F; ssm_au_c=kvugCAFOkIBXi0GEjgNZn6TNy90ybsUSkv2eNav5S3eYgAAAAiQmijAl3kNEDFP3PujtRVnGdaAXPZgjENQwJbu5oJP0=; _ga=GA1.1.1932356187.1600157327; _ga_7VKFYR6RV1=GS1.1.1605163485.154.0.1605163485.60; page_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; spage_uid=UI05gdp0YidssBiwDL0ssssssGK-466077; ncpa=221844|kh44u848|395aa407aa9c951d73d8de3fa3ce656c5d6ef428|s_1a7f4dd73489|97a684e827d8975db0e10abff1118b51d7a85ffa:1101468|kh44vds8|ff681b362b8a6666119d0a169ff8e92f5df344a5|s_1b3802fd63cf|f75d2ecf6b99d17f40a5a4692358db9995a2dac8:845657|kh45wqow|5cad2ef28fafd769103a495fa86c4510ccd30c82|s_54853016347d|9e6dc8c0e97a9ab511f0b55a0ba1cd5db2522760:1860038|kh460qzc|50fcd1ac9e51eaf79df8b38dd9bdc0845f0f45ab|s_15cb275e34f04|f35a46ca9e41df390bd03642eaa42afa19f65ed9:887927|kh46dqko|3564b8a8982890613b5ff90d5c68f8fc5e4a55ca|s_1b23e96d6b1fd|718cbd82b224a98a5bb26fd98401b6e40856b4f2:197023|kh46fdzk|89778e72078a60264cc317a63f523ef2a1090634|s_1a7f4b55d0bb|142c9e76770c86f037d1d76e2ce8f00123dbb8ef:24|kh46h9w0|514e6e49616c349dc94d31b9a85cd9a43485113d|s_419afe53a6bb|1f0c44bb64e6ca64f62753fde0a6e9a30d925da0:17703|kh5yj708|1b94217d27ff92d18e091e4b26be526631f2b666|s_1f0b6dd345b2|8da79206b3c0d93283e34b5f8e2e5540b8a420ff:95694|khboay0o|1ef5206f40b2fca16c0e50336107342771fd4d61|null|9eef7fd400ec779739dac15e7bef385ebdd0326f:692492|kheq2nlc|14e7f0c8a5cb417eecc3ba4821698bd8fdcd3b64|s_a072289e9d4f|414aa3c087e4b7cefb044f78174600558dc93cf7' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/6999016004/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=10900&amp;nvMid=6999016004&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20013178&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.141 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/6999016004?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; NID_SES=AAABnJRDbhBfyvobBHn7LYxr5Zn8Y2kJOXY2oDhkF3IoN7UW5hPP8DQT4iuqa651AbPPw5lF4Uzh/gSyuUmiXW39nkY7MkaS+0e/7BLwEzuLsP0SaDhDUtDOWj+p2DjRxq87Mm0fKSefD+75wAtMWuofTp5joTO42Vszy10KzONx7MZjUBVn6eq0dz4zh6pnQwm2b2yAidZlweAJGSRKm66OyMAZputPcv3xuO5PSbh/udhHh0FQ4ati1ywTadjytC/Mi/k5EFYxH1bDijby2Au1vC15g1SlCYBQ7HjTDsUUHpwTWVqElJ6pcXENTJesJpOILu+OOo+D1O/XAVXkYdtAg9B1PDMSC8H5lcX2UmMxmtbLuu0NdYoQyzcijpFzQBJrjPA0A3cZrvgy2sHQJNAfBC1Ss+phxrz+t6pkVDJc08PK1rmOea/cj2X9kCaMscak2ylCMSFfyIzbi7+NzufQInHNUxJ569agfaXX43DleU38BWwb+RfDauZyQpuLgchK8rI3nL0Nkuhft0Fmzh2NIl+v9F8BuIbFQQFuD0K+lGus; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/16654052240/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=16900&amp;nvMid=16654052240&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20056401&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.141 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/16654052240?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; NID_SES=AAABnJRDbhBfyvobBHn7LYxr5Zn8Y2kJOXY2oDhkF3IoN7UW5hPP8DQT4iuqa651AbPPw5lF4Uzh/gSyuUmiXW39nkY7MkaS+0e/7BLwEzuLsP0SaDhDUtDOWj+p2DjRxq87Mm0fKSefD+75wAtMWuofTp5joTO42Vszy10KzONx7MZjUBVn6eq0dz4zh6pnQwm2b2yAidZlweAJGSRKm66OyMAZputPcv3xuO5PSbh/udhHh0FQ4ati1ywTadjytC/Mi/k5EFYxH1bDijby2Au1vC15g1SlCYBQ7HjTDsUUHpwTWVqElJ6pcXENTJesJpOILu+OOo+D1O/XAVXkYdtAg9B1PDMSC8H5lcX2UmMxmtbLuu0NdYoQyzcijpFzQBJrjPA0A3cZrvgy2sHQJNAfBC1Ss+phxrz+t6pkVDJc08PK1rmOea/cj2X9kCaMscak2ylCMSFfyIzbi7+NzufQInHNUxJ569agfaXX43DleU38BWwb+RfDauZyQpuLgchK8rI3nL0Nkuhft0Fmzh2NIl+v9F8BuIbFQQFuD0K+lGus; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/13057454748/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=14400&amp;nvMid=13057454748&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20040506&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.141 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/13057454748?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; NID_SES=AAABnJRDbhBfyvobBHn7LYxr5Zn8Y2kJOXY2oDhkF3IoN7UW5hPP8DQT4iuqa651AbPPw5lF4Uzh/gSyuUmiXW39nkY7MkaS+0e/7BLwEzuLsP0SaDhDUtDOWj+p2DjRxq87Mm0fKSefD+75wAtMWuofTp5joTO42Vszy10KzONx7MZjUBVn6eq0dz4zh6pnQwm2b2yAidZlweAJGSRKm66OyMAZputPcv3xuO5PSbh/udhHh0FQ4ati1ywTadjytC/Mi/k5EFYxH1bDijby2Au1vC15g1SlCYBQ7HjTDsUUHpwTWVqElJ6pcXENTJesJpOILu+OOo+D1O/XAVXkYdtAg9B1PDMSC8H5lcX2UmMxmtbLuu0NdYoQyzcijpFzQBJrjPA0A3cZrvgy2sHQJNAfBC1Ss+phxrz+t6pkVDJc08PK1rmOea/cj2X9kCaMscak2ylCMSFfyIzbi7+NzufQInHNUxJ569agfaXX43DleU38BWwb+RfDauZyQpuLgchK8rI3nL0Nkuhft0Fmzh2NIl+v9F8BuIbFQQFuD0K+lGus; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/6512752936/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=15180&amp;nvMid=6512752936&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20040506&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.141 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/6512752936?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; NID_SES=AAABnJRDbhBfyvobBHn7LYxr5Zn8Y2kJOXY2oDhkF3IoN7UW5hPP8DQT4iuqa651AbPPw5lF4Uzh/gSyuUmiXW39nkY7MkaS+0e/7BLwEzuLsP0SaDhDUtDOWj+p2DjRxq87Mm0fKSefD+75wAtMWuofTp5joTO42Vszy10KzONx7MZjUBVn6eq0dz4zh6pnQwm2b2yAidZlweAJGSRKm66OyMAZputPcv3xuO5PSbh/udhHh0FQ4ati1ywTadjytC/Mi/k5EFYxH1bDijby2Au1vC15g1SlCYBQ7HjTDsUUHpwTWVqElJ6pcXENTJesJpOILu+OOo+D1O/XAVXkYdtAg9B1PDMSC8H5lcX2UmMxmtbLuu0NdYoQyzcijpFzQBJrjPA0A3cZrvgy2sHQJNAfBC1Ss+phxrz+t6pkVDJc08PK1rmOea/cj2X9kCaMscak2ylCMSFfyIzbi7+NzufQInHNUxJ569agfaXX43DleU38BWwb+RfDauZyQpuLgchK8rI3nL0Nkuhft0Fmzh2NIl+v9F8BuIbFQQFuD0K+lGus; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/9803321078/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=25720&amp;nvMid=9803321078&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20040510&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.141 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/9803321078?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; NID_SES=AAABnJRDbhBfyvobBHn7LYxr5Zn8Y2kJOXY2oDhkF3IoN7UW5hPP8DQT4iuqa651AbPPw5lF4Uzh/gSyuUmiXW39nkY7MkaS+0e/7BLwEzuLsP0SaDhDUtDOWj+p2DjRxq87Mm0fKSefD+75wAtMWuofTp5joTO42Vszy10KzONx7MZjUBVn6eq0dz4zh6pnQwm2b2yAidZlweAJGSRKm66OyMAZputPcv3xuO5PSbh/udhHh0FQ4ati1ywTadjytC/Mi/k5EFYxH1bDijby2Au1vC15g1SlCYBQ7HjTDsUUHpwTWVqElJ6pcXENTJesJpOILu+OOo+D1O/XAVXkYdtAg9B1PDMSC8H5lcX2UmMxmtbLuu0NdYoQyzcijpFzQBJrjPA0A3cZrvgy2sHQJNAfBC1Ss+phxrz+t6pkVDJc08PK1rmOea/cj2X9kCaMscak2ylCMSFfyIzbi7+NzufQInHNUxJ569agfaXX43DleU38BWwb+RfDauZyQpuLgchK8rI3nL0Nkuhft0Fmzh2NIl+v9F8BuIbFQQFuD0K+lGus; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/9803321078/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=14980&amp;nvMid=9803321078&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20040506&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.141 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/9803321078?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; NID_SES=AAABnJRDbhBfyvobBHn7LYxr5Zn8Y2kJOXY2oDhkF3IoN7UW5hPP8DQT4iuqa651AbPPw5lF4Uzh/gSyuUmiXW39nkY7MkaS+0e/7BLwEzuLsP0SaDhDUtDOWj+p2DjRxq87Mm0fKSefD+75wAtMWuofTp5joTO42Vszy10KzONx7MZjUBVn6eq0dz4zh6pnQwm2b2yAidZlweAJGSRKm66OyMAZputPcv3xuO5PSbh/udhHh0FQ4ati1ywTadjytC/Mi/k5EFYxH1bDijby2Au1vC15g1SlCYBQ7HjTDsUUHpwTWVqElJ6pcXENTJesJpOILu+OOo+D1O/XAVXkYdtAg9B1PDMSC8H5lcX2UmMxmtbLuu0NdYoQyzcijpFzQBJrjPA0A3cZrvgy2sHQJNAfBC1Ss+phxrz+t6pkVDJc08PK1rmOea/cj2X9kCaMscak2ylCMSFfyIzbi7+NzufQInHNUxJ569agfaXX43DleU38BWwb+RfDauZyQpuLgchK8rI3nL0Nkuhft0Fmzh2NIl+v9F8BuIbFQQFuD0K+lGus; spage_uid=' \
+  --compressed</t>
+  </si>
+  <si>
+    <t>curl 'https://search.shopping.naver.com/catalog/21151605555/products-by-mall?cardPrice=false&amp;deliveryToday=false&amp;isNPayPlus=false&amp;lowestPrice=16930&amp;nvMid=21151605555&amp;onlyBeautyWindow=false&amp;page=1&amp;pageSize=7&amp;pr=PC&amp;purchaseConditionSeq1=20040506&amp;sort=LOW_PRICE&amp;withFee=false&amp;isManual=true&amp;catalogProviderTypeCode=P13001&amp;exposeAreaName=SUMMARY_PRODUCTS_BY_MALL_PRICE&amp;catalogType=BRAND&amp;inflow=brc' \
+  -H 'Connection: keep-alive' \
+  -H 'Accept: application/json, text/plain, */*' \
+  -H 'User-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/87.0.4280.141 Safari/537.36' \
+  -H 'urlprefix: /api' \
+  -H 'Sec-Fetch-Site: same-origin' \
+  -H 'Sec-Fetch-Mode: cors' \
+  -H 'Sec-Fetch-Dest: empty' \
+  -H 'Referer: https://search.shopping.naver.com/catalog/21151605555?' \
+  -H 'Accept-Language: en-US,en;q=0.9' \
+  -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; NID_SES=AAABnJRDbhBfyvobBHn7LYxr5Zn8Y2kJOXY2oDhkF3IoN7UW5hPP8DQT4iuqa651AbPPw5lF4Uzh/gSyuUmiXW39nkY7MkaS+0e/7BLwEzuLsP0SaDhDUtDOWj+p2DjRxq87Mm0fKSefD+75wAtMWuofTp5joTO42Vszy10KzONx7MZjUBVn6eq0dz4zh6pnQwm2b2yAidZlweAJGSRKm66OyMAZputPcv3xuO5PSbh/udhHh0FQ4ati1ywTadjytC/Mi/k5EFYxH1bDijby2Au1vC15g1SlCYBQ7HjTDsUUHpwTWVqElJ6pcXENTJesJpOILu+OOo+D1O/XAVXkYdtAg9B1PDMSC8H5lcX2UmMxmtbLuu0NdYoQyzcijpFzQBJrjPA0A3cZrvgy2sHQJNAfBC1Ss+phxrz+t6pkVDJc08PK1rmOea/cj2X9kCaMscak2ylCMSFfyIzbi7+NzufQInHNUxJ569agfaXX43DleU38BWwb+RfDauZyQpuLgchK8rI3nL0Nkuhft0Fmzh2NIl+v9F8BuIbFQQFuD0K+lGus; spage_uid=' \
   --compressed</t>
   </si>
 </sst>
@@ -5538,8 +5594,11 @@
     <xf numFmtId="0" fontId="16" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5588,9 +5647,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="41">
@@ -7345,10 +7401,10 @@
   <dimension ref="A1:BJ81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="11" topLeftCell="L44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="11" topLeftCell="M48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="N50" sqref="N50"/>
+      <selection pane="bottomRight" activeCell="M67" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -7500,10 +7556,10 @@
       <c r="X8" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="Y8" s="75" t="s">
+      <c r="Y8" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="Z8" s="75"/>
+      <c r="Z8" s="76"/>
       <c r="AA8" s="8"/>
       <c r="AB8" s="8"/>
       <c r="AC8" s="8"/>
@@ -7559,155 +7615,155 @@
     </row>
     <row r="9" spans="1:62" ht="15.75">
       <c r="A9" s="7"/>
-      <c r="B9" s="76" t="s">
+      <c r="B9" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="77"/>
-      <c r="K9" s="77"/>
-      <c r="L9" s="77"/>
-      <c r="M9" s="77"/>
-      <c r="N9" s="77"/>
-      <c r="O9" s="77"/>
-      <c r="P9" s="77"/>
-      <c r="Q9" s="77"/>
-      <c r="R9" s="77"/>
-      <c r="S9" s="77"/>
-      <c r="T9" s="77"/>
-      <c r="U9" s="77"/>
-      <c r="V9" s="77"/>
-      <c r="W9" s="77"/>
-      <c r="X9" s="77"/>
-      <c r="Y9" s="77"/>
-      <c r="Z9" s="78"/>
-      <c r="AA9" s="79" t="s">
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="78"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="78"/>
+      <c r="P9" s="78"/>
+      <c r="Q9" s="78"/>
+      <c r="R9" s="78"/>
+      <c r="S9" s="78"/>
+      <c r="T9" s="78"/>
+      <c r="U9" s="78"/>
+      <c r="V9" s="78"/>
+      <c r="W9" s="78"/>
+      <c r="X9" s="78"/>
+      <c r="Y9" s="78"/>
+      <c r="Z9" s="79"/>
+      <c r="AA9" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="AB9" s="80"/>
-      <c r="AC9" s="80"/>
-      <c r="AD9" s="80"/>
-      <c r="AE9" s="80"/>
-      <c r="AF9" s="80"/>
-      <c r="AG9" s="80"/>
-      <c r="AH9" s="80"/>
-      <c r="AI9" s="80"/>
-      <c r="AJ9" s="80"/>
-      <c r="AK9" s="80"/>
-      <c r="AL9" s="80"/>
-      <c r="AM9" s="80"/>
-      <c r="AN9" s="80"/>
-      <c r="AO9" s="80"/>
-      <c r="AP9" s="80"/>
-      <c r="AQ9" s="80"/>
-      <c r="AR9" s="81"/>
-      <c r="AS9" s="82" t="s">
+      <c r="AB9" s="81"/>
+      <c r="AC9" s="81"/>
+      <c r="AD9" s="81"/>
+      <c r="AE9" s="81"/>
+      <c r="AF9" s="81"/>
+      <c r="AG9" s="81"/>
+      <c r="AH9" s="81"/>
+      <c r="AI9" s="81"/>
+      <c r="AJ9" s="81"/>
+      <c r="AK9" s="81"/>
+      <c r="AL9" s="81"/>
+      <c r="AM9" s="81"/>
+      <c r="AN9" s="81"/>
+      <c r="AO9" s="81"/>
+      <c r="AP9" s="81"/>
+      <c r="AQ9" s="81"/>
+      <c r="AR9" s="82"/>
+      <c r="AS9" s="83" t="s">
         <v>135</v>
       </c>
-      <c r="AT9" s="83"/>
-      <c r="AU9" s="83"/>
-      <c r="AV9" s="83"/>
-      <c r="AW9" s="83"/>
-      <c r="AX9" s="83"/>
-      <c r="AY9" s="83"/>
-      <c r="AZ9" s="83"/>
-      <c r="BA9" s="83"/>
-      <c r="BB9" s="83"/>
-      <c r="BC9" s="83"/>
-      <c r="BD9" s="83"/>
-      <c r="BE9" s="83"/>
-      <c r="BF9" s="83"/>
-      <c r="BG9" s="83"/>
-      <c r="BH9" s="83"/>
-      <c r="BI9" s="83"/>
-      <c r="BJ9" s="84"/>
+      <c r="AT9" s="84"/>
+      <c r="AU9" s="84"/>
+      <c r="AV9" s="84"/>
+      <c r="AW9" s="84"/>
+      <c r="AX9" s="84"/>
+      <c r="AY9" s="84"/>
+      <c r="AZ9" s="84"/>
+      <c r="BA9" s="84"/>
+      <c r="BB9" s="84"/>
+      <c r="BC9" s="84"/>
+      <c r="BD9" s="84"/>
+      <c r="BE9" s="84"/>
+      <c r="BF9" s="84"/>
+      <c r="BG9" s="84"/>
+      <c r="BH9" s="84"/>
+      <c r="BI9" s="84"/>
+      <c r="BJ9" s="85"/>
     </row>
     <row r="10" spans="1:62">
       <c r="A10" s="4"/>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="86" t="s">
         <v>314</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="73" t="s">
+      <c r="C10" s="87"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="74" t="s">
+      <c r="K10" s="74"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="R10" s="74"/>
-      <c r="S10" s="74"/>
-      <c r="T10" s="74"/>
-      <c r="U10" s="74"/>
-      <c r="V10" s="74"/>
-      <c r="W10" s="74"/>
-      <c r="X10" s="74"/>
-      <c r="Y10" s="74"/>
-      <c r="Z10" s="74"/>
-      <c r="AA10" s="72" t="s">
+      <c r="R10" s="75"/>
+      <c r="S10" s="75"/>
+      <c r="T10" s="75"/>
+      <c r="U10" s="75"/>
+      <c r="V10" s="75"/>
+      <c r="W10" s="75"/>
+      <c r="X10" s="75"/>
+      <c r="Y10" s="75"/>
+      <c r="Z10" s="75"/>
+      <c r="AA10" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="AB10" s="72"/>
-      <c r="AC10" s="72"/>
-      <c r="AD10" s="72"/>
-      <c r="AE10" s="72"/>
-      <c r="AF10" s="73" t="s">
+      <c r="AB10" s="73"/>
+      <c r="AC10" s="73"/>
+      <c r="AD10" s="73"/>
+      <c r="AE10" s="73"/>
+      <c r="AF10" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="AG10" s="73"/>
-      <c r="AH10" s="73"/>
-      <c r="AI10" s="73"/>
-      <c r="AJ10" s="73"/>
-      <c r="AK10" s="73"/>
-      <c r="AL10" s="74" t="s">
+      <c r="AG10" s="74"/>
+      <c r="AH10" s="74"/>
+      <c r="AI10" s="74"/>
+      <c r="AJ10" s="74"/>
+      <c r="AK10" s="74"/>
+      <c r="AL10" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="AM10" s="74"/>
-      <c r="AN10" s="74"/>
-      <c r="AO10" s="74"/>
-      <c r="AP10" s="74"/>
-      <c r="AQ10" s="74"/>
-      <c r="AR10" s="74"/>
-      <c r="AS10" s="72" t="s">
+      <c r="AM10" s="75"/>
+      <c r="AN10" s="75"/>
+      <c r="AO10" s="75"/>
+      <c r="AP10" s="75"/>
+      <c r="AQ10" s="75"/>
+      <c r="AR10" s="75"/>
+      <c r="AS10" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="AT10" s="72"/>
-      <c r="AU10" s="72"/>
-      <c r="AV10" s="72"/>
-      <c r="AW10" s="72"/>
-      <c r="AX10" s="73" t="s">
+      <c r="AT10" s="73"/>
+      <c r="AU10" s="73"/>
+      <c r="AV10" s="73"/>
+      <c r="AW10" s="73"/>
+      <c r="AX10" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="AY10" s="73"/>
-      <c r="AZ10" s="73"/>
-      <c r="BA10" s="73"/>
-      <c r="BB10" s="73"/>
-      <c r="BC10" s="73"/>
-      <c r="BD10" s="74" t="s">
+      <c r="AY10" s="74"/>
+      <c r="AZ10" s="74"/>
+      <c r="BA10" s="74"/>
+      <c r="BB10" s="74"/>
+      <c r="BC10" s="74"/>
+      <c r="BD10" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="BE10" s="74"/>
-      <c r="BF10" s="74"/>
-      <c r="BG10" s="74"/>
-      <c r="BH10" s="74"/>
-      <c r="BI10" s="74"/>
-      <c r="BJ10" s="74"/>
+      <c r="BE10" s="75"/>
+      <c r="BF10" s="75"/>
+      <c r="BG10" s="75"/>
+      <c r="BH10" s="75"/>
+      <c r="BI10" s="75"/>
+      <c r="BJ10" s="75"/>
     </row>
     <row r="11" spans="1:62">
       <c r="A11" s="10" t="s">
@@ -8244,8 +8300,8 @@
       <c r="L16" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="M16" s="34" t="s">
-        <v>563</v>
+      <c r="M16" s="71" t="s">
+        <v>777</v>
       </c>
       <c r="N16" s="16">
         <v>1000</v>
@@ -8323,7 +8379,7 @@
         <v>170</v>
       </c>
       <c r="M17" s="34" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="N17" s="16">
         <v>1000</v>
@@ -8401,7 +8457,7 @@
         <v>173</v>
       </c>
       <c r="M18" s="34" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="N18" s="16">
         <v>1000</v>
@@ -8479,7 +8535,7 @@
         <v>176</v>
       </c>
       <c r="M19" s="34" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="N19" s="16">
         <v>1600</v>
@@ -8557,7 +8613,7 @@
         <v>179</v>
       </c>
       <c r="M20" s="34" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="N20" s="16">
         <v>2000</v>
@@ -8714,7 +8770,7 @@
       <c r="L22" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="M22" s="34"/>
+      <c r="M22" s="71"/>
       <c r="N22" s="16">
         <v>370</v>
       </c>
@@ -8792,7 +8848,7 @@
       <c r="L23" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="M23" s="34"/>
+      <c r="M23" s="72"/>
       <c r="N23" s="16">
         <v>370</v>
       </c>
@@ -9183,7 +9239,7 @@
       <c r="L28" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="M28" s="34"/>
+      <c r="M28" s="71"/>
       <c r="N28" s="16">
         <v>275</v>
       </c>
@@ -9261,7 +9317,7 @@
       <c r="L29" s="35" t="s">
         <v>215</v>
       </c>
-      <c r="M29" s="34"/>
+      <c r="M29" s="71"/>
       <c r="N29" s="16">
         <v>900</v>
       </c>
@@ -9339,7 +9395,7 @@
       <c r="L30" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="M30" s="34"/>
+      <c r="M30" s="72"/>
       <c r="N30" s="16">
         <v>6</v>
       </c>
@@ -9417,7 +9473,7 @@
       <c r="L31" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="M31" s="34"/>
+      <c r="M31" s="71"/>
       <c r="N31" s="16">
         <v>2.2000000000000002</v>
       </c>
@@ -9493,8 +9549,8 @@
       <c r="L32" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="M32" s="34" t="s">
-        <v>568</v>
+      <c r="M32" s="71" t="s">
+        <v>567</v>
       </c>
       <c r="N32" s="16">
         <v>8</v>
@@ -9574,8 +9630,8 @@
       <c r="L33" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="M33" s="34" t="s">
-        <v>568</v>
+      <c r="M33" s="71" t="s">
+        <v>779</v>
       </c>
       <c r="N33" s="16">
         <v>4</v>
@@ -9655,8 +9711,8 @@
       <c r="L34" s="27" t="s">
         <v>231</v>
       </c>
-      <c r="M34" s="34" t="s">
-        <v>569</v>
+      <c r="M34" s="71" t="s">
+        <v>568</v>
       </c>
       <c r="N34" s="16">
         <v>8</v>
@@ -9736,8 +9792,8 @@
       <c r="L35" s="27" t="s">
         <v>231</v>
       </c>
-      <c r="M35" s="34" t="s">
-        <v>569</v>
+      <c r="M35" s="71" t="s">
+        <v>780</v>
       </c>
       <c r="N35" s="16">
         <v>4</v>
@@ -9817,8 +9873,8 @@
       <c r="L36" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="M36" s="34" t="s">
-        <v>570</v>
+      <c r="M36" s="71" t="s">
+        <v>781</v>
       </c>
       <c r="N36" s="16">
         <v>8</v>
@@ -9898,8 +9954,8 @@
       <c r="L37" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="M37" s="34" t="s">
-        <v>570</v>
+      <c r="M37" s="71" t="s">
+        <v>782</v>
       </c>
       <c r="N37" s="16">
         <v>4</v>
@@ -9979,8 +10035,8 @@
       <c r="L38" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="M38" s="34" t="s">
-        <v>571</v>
+      <c r="M38" s="71" t="s">
+        <v>783</v>
       </c>
       <c r="N38" s="16">
         <v>4</v>
@@ -10060,8 +10116,8 @@
       <c r="L39" s="27" t="s">
         <v>454</v>
       </c>
-      <c r="M39" s="34" t="s">
-        <v>572</v>
+      <c r="M39" s="71" t="s">
+        <v>778</v>
       </c>
       <c r="N39" s="16">
         <v>2</v>
@@ -10142,8 +10198,8 @@
       <c r="L40" s="27" t="s">
         <v>241</v>
       </c>
-      <c r="M40" s="34" t="s">
-        <v>573</v>
+      <c r="M40" s="71" t="s">
+        <v>570</v>
       </c>
       <c r="N40" s="16">
         <v>1</v>
@@ -10224,8 +10280,8 @@
       <c r="L41" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="M41" s="34" t="s">
-        <v>574</v>
+      <c r="M41" s="71" t="s">
+        <v>571</v>
       </c>
       <c r="N41" s="16">
         <v>2</v>
@@ -10306,8 +10362,8 @@
       <c r="L42" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="M42" s="34" t="s">
-        <v>575</v>
+      <c r="M42" s="71" t="s">
+        <v>572</v>
       </c>
       <c r="N42" s="16">
         <v>2</v>
@@ -10388,11 +10444,11 @@
       <c r="L43" s="27" t="s">
         <v>249</v>
       </c>
-      <c r="M43" s="34" t="s">
-        <v>576</v>
+      <c r="M43" s="71" t="s">
+        <v>573</v>
       </c>
       <c r="N43" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O43" s="44" t="s">
         <v>461</v>
@@ -10470,8 +10526,8 @@
       <c r="L44" s="27" t="s">
         <v>454</v>
       </c>
-      <c r="M44" s="34" t="s">
-        <v>572</v>
+      <c r="M44" s="71" t="s">
+        <v>569</v>
       </c>
       <c r="N44" s="16">
         <v>1</v>
@@ -10554,8 +10610,8 @@
       <c r="L45" s="27" t="s">
         <v>255</v>
       </c>
-      <c r="M45" s="34" t="s">
-        <v>577</v>
+      <c r="M45" s="71" t="s">
+        <v>574</v>
       </c>
       <c r="N45" s="16">
         <v>1</v>
@@ -10638,8 +10694,8 @@
       <c r="L46" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="M46" s="34" t="s">
-        <v>578</v>
+      <c r="M46" s="71" t="s">
+        <v>575</v>
       </c>
       <c r="N46" s="16">
         <v>1</v>
@@ -10723,8 +10779,8 @@
       <c r="L47" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="M47" s="88" t="s">
-        <v>779</v>
+      <c r="M47" s="71" t="s">
+        <v>776</v>
       </c>
       <c r="N47" s="16">
         <v>1</v>
@@ -10809,7 +10865,7 @@
         <v>263</v>
       </c>
       <c r="M48" s="34" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="N48" s="16">
         <v>1</v>
@@ -10894,7 +10950,7 @@
         <v>267</v>
       </c>
       <c r="M49" s="34" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="N49" s="16">
         <v>1</v>
@@ -11061,7 +11117,7 @@
         <v>270</v>
       </c>
       <c r="M51" s="34" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="N51" s="16">
         <v>1</v>
@@ -11146,7 +11202,7 @@
         <v>273</v>
       </c>
       <c r="M52" s="34" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="N52" s="16">
         <v>4</v>
@@ -11230,7 +11286,7 @@
         <v>276</v>
       </c>
       <c r="M53" s="34" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="N53" s="16">
         <v>6</v>
@@ -11315,7 +11371,7 @@
         <v>278</v>
       </c>
       <c r="M54" s="34" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="N54" s="16">
         <v>6</v>
@@ -11400,7 +11456,7 @@
         <v>281</v>
       </c>
       <c r="M55" s="34" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="N55" s="16">
         <v>1</v>
@@ -11482,7 +11538,7 @@
         <v>482</v>
       </c>
       <c r="M56" s="34" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="N56" s="17">
         <v>2800</v>
@@ -11559,7 +11615,7 @@
         <v>492</v>
       </c>
       <c r="M57" s="34" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="N57" s="17">
         <v>1900</v>
@@ -11636,7 +11692,7 @@
         <v>498</v>
       </c>
       <c r="M58" s="34" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="N58" s="17">
         <v>2000</v>
@@ -11713,7 +11769,7 @@
         <v>508</v>
       </c>
       <c r="M59" s="34" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="N59" s="17">
         <v>2800</v>
@@ -11790,7 +11846,7 @@
         <v>514</v>
       </c>
       <c r="M60" s="34" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="N60" s="17">
         <v>1900</v>
@@ -11867,7 +11923,7 @@
         <v>520</v>
       </c>
       <c r="M61" s="34" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="N61" s="17">
         <v>2000</v>
@@ -11944,7 +12000,7 @@
         <v>530</v>
       </c>
       <c r="M62" s="34" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="N62" s="17">
         <v>2800</v>
@@ -12021,7 +12077,7 @@
         <v>536</v>
       </c>
       <c r="M63" s="34" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="N63" s="17">
         <v>1900</v>
@@ -12063,30 +12119,30 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="64" spans="1:29" ht="409.5">
+    <row r="64" spans="1:29">
       <c r="A64" s="17">
         <v>53</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="E64" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G64" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H64" s="17" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="I64" s="17">
         <v>1</v>
@@ -12095,43 +12151,43 @@
         <v>9606247018</v>
       </c>
       <c r="K64" s="17" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="M64" s="71" t="s">
-        <v>761</v>
+        <v>650</v>
+      </c>
+      <c r="M64" s="65" t="s">
+        <v>758</v>
       </c>
       <c r="N64" s="17">
         <v>184</v>
       </c>
       <c r="O64" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P64" s="17">
         <v>1</v>
       </c>
       <c r="Q64" s="17" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="R64" s="17" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="S64" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T64" s="17" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="U64" s="17" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="V64" s="17">
         <v>46</v>
       </c>
       <c r="W64" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X64" s="17">
         <v>4</v>
@@ -12143,30 +12199,30 @@
         <v>60900</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="409.5">
+    <row r="65" spans="1:26">
       <c r="A65" s="17">
         <v>54</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G65" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H65" s="17" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="I65" s="17">
         <v>2</v>
@@ -12175,43 +12231,43 @@
         <v>21798278124</v>
       </c>
       <c r="K65" s="17" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="M65" s="71" t="s">
-        <v>762</v>
+        <v>652</v>
+      </c>
+      <c r="M65" s="65" t="s">
+        <v>759</v>
       </c>
       <c r="N65" s="17">
         <v>168</v>
       </c>
       <c r="O65" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P65" s="17">
         <v>1</v>
       </c>
       <c r="Q65" s="17" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="R65" s="17" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="S65" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T65" s="17" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="U65" s="17" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="V65" s="17">
         <v>42</v>
       </c>
       <c r="W65" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X65" s="17">
         <v>4</v>
@@ -12223,30 +12279,30 @@
         <v>60900</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="409.5">
+    <row r="66" spans="1:26">
       <c r="A66" s="17">
         <v>55</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="E66" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G66" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H66" s="17" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="I66" s="17">
         <v>3</v>
@@ -12255,43 +12311,43 @@
         <v>20804055294</v>
       </c>
       <c r="K66" s="17" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="M66" s="71" t="s">
-        <v>763</v>
+        <v>654</v>
+      </c>
+      <c r="M66" s="65" t="s">
+        <v>760</v>
       </c>
       <c r="N66" s="17">
         <v>144</v>
       </c>
       <c r="O66" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P66" s="17">
         <v>1</v>
       </c>
       <c r="Q66" s="17" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="R66" s="17" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="S66" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T66" s="17" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="U66" s="17" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="V66" s="17">
         <v>36</v>
       </c>
       <c r="W66" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X66" s="17">
         <v>4</v>
@@ -12303,30 +12359,30 @@
         <v>60900</v>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="409.5">
+    <row r="67" spans="1:26">
       <c r="A67" s="17">
         <v>56</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="E67" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F67" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G67" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H67" s="17" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="I67" s="17">
         <v>4</v>
@@ -12335,43 +12391,43 @@
         <v>20804087696</v>
       </c>
       <c r="K67" s="17" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="M67" s="71" t="s">
-        <v>764</v>
+        <v>656</v>
+      </c>
+      <c r="M67" s="65" t="s">
+        <v>761</v>
       </c>
       <c r="N67" s="17">
         <v>112</v>
       </c>
       <c r="O67" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P67" s="17">
         <v>1</v>
       </c>
       <c r="Q67" s="17" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="R67" s="17" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="S67" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T67" s="17" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="U67" s="17" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="V67" s="17">
         <v>28</v>
       </c>
       <c r="W67" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X67" s="17">
         <v>4</v>
@@ -12383,30 +12439,30 @@
         <v>60900</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="409.5">
+    <row r="68" spans="1:26">
       <c r="A68" s="17">
         <v>57</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E68" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G68" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H68" s="17" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="I68" s="17">
         <v>5</v>
@@ -12415,43 +12471,43 @@
         <v>24355155523</v>
       </c>
       <c r="K68" s="17" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="M68" s="71" t="s">
-        <v>765</v>
+        <v>658</v>
+      </c>
+      <c r="M68" s="65" t="s">
+        <v>762</v>
       </c>
       <c r="N68" s="17">
         <v>120</v>
       </c>
       <c r="O68" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P68" s="17">
         <v>1</v>
       </c>
       <c r="Q68" s="17" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="R68" s="17" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="S68" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T68" s="17" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="U68" s="17" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="V68" s="17">
         <v>30</v>
       </c>
       <c r="W68" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X68" s="17">
         <v>4</v>
@@ -12463,30 +12519,30 @@
         <v>50900</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="409.5">
+    <row r="69" spans="1:26">
       <c r="A69" s="17">
         <v>58</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="E69" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G69" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H69" s="17" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="I69" s="17">
         <v>6</v>
@@ -12495,43 +12551,43 @@
         <v>24355221522</v>
       </c>
       <c r="K69" s="17" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="M69" s="71" t="s">
-        <v>766</v>
+        <v>660</v>
+      </c>
+      <c r="M69" s="65" t="s">
+        <v>763</v>
       </c>
       <c r="N69" s="17">
         <v>104</v>
       </c>
       <c r="O69" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P69" s="17">
         <v>1</v>
       </c>
       <c r="Q69" s="17" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="R69" s="17" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="S69" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T69" s="17" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="U69" s="17" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="V69" s="17">
         <v>26</v>
       </c>
       <c r="W69" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X69" s="17">
         <v>4</v>
@@ -12543,30 +12599,30 @@
         <v>50900</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="409.5">
+    <row r="70" spans="1:26">
       <c r="A70" s="17">
         <v>59</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E70" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G70" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H70" s="17" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="I70" s="17">
         <v>7</v>
@@ -12575,43 +12631,43 @@
         <v>24355278522</v>
       </c>
       <c r="K70" s="17" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="M70" s="71" t="s">
-        <v>767</v>
+        <v>662</v>
+      </c>
+      <c r="M70" s="65" t="s">
+        <v>764</v>
       </c>
       <c r="N70" s="17">
         <v>88</v>
       </c>
       <c r="O70" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P70" s="17">
         <v>1</v>
       </c>
       <c r="Q70" s="17" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="R70" s="17" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="S70" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T70" s="17" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="U70" s="17" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="V70" s="17">
         <v>22</v>
       </c>
       <c r="W70" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X70" s="17">
         <v>4</v>
@@ -12623,30 +12679,30 @@
         <v>50900</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="409.5">
+    <row r="71" spans="1:26">
       <c r="A71" s="17">
         <v>60</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="E71" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G71" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I71" s="17">
         <v>8</v>
@@ -12655,43 +12711,43 @@
         <v>21800768787</v>
       </c>
       <c r="K71" s="17" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="M71" s="71" t="s">
-        <v>768</v>
+        <v>664</v>
+      </c>
+      <c r="M71" s="65" t="s">
+        <v>765</v>
       </c>
       <c r="N71" s="17">
         <v>186</v>
       </c>
       <c r="O71" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P71" s="17">
         <v>1</v>
       </c>
       <c r="Q71" s="17" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="R71" s="17" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="S71" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T71" s="17" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="U71" s="17" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="V71" s="17">
         <v>186</v>
       </c>
       <c r="W71" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X71" s="17">
         <v>1</v>
@@ -12703,30 +12759,30 @@
         <v>54500</v>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="409.5">
+    <row r="72" spans="1:26">
       <c r="A72" s="17">
         <v>61</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D72" s="17" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="E72" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G72" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H72" s="17" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I72" s="17">
         <v>9</v>
@@ -12735,43 +12791,43 @@
         <v>21800772029</v>
       </c>
       <c r="K72" s="17" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="M72" s="71" t="s">
-        <v>769</v>
+        <v>666</v>
+      </c>
+      <c r="M72" s="65" t="s">
+        <v>766</v>
       </c>
       <c r="N72" s="17">
         <v>168</v>
       </c>
       <c r="O72" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P72" s="17">
         <v>1</v>
       </c>
       <c r="Q72" s="17" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="R72" s="17" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="S72" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T72" s="17" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="U72" s="17" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="V72" s="17">
         <v>168</v>
       </c>
       <c r="W72" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X72" s="17">
         <v>1</v>
@@ -12783,30 +12839,30 @@
         <v>54500</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="409.5">
+    <row r="73" spans="1:26">
       <c r="A73" s="17">
         <v>62</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="E73" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G73" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H73" s="17" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I73" s="17">
         <v>10</v>
@@ -12815,43 +12871,43 @@
         <v>21799603401</v>
       </c>
       <c r="K73" s="17" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="M73" s="71" t="s">
-        <v>770</v>
+        <v>668</v>
+      </c>
+      <c r="M73" s="65" t="s">
+        <v>767</v>
       </c>
       <c r="N73" s="17">
         <v>150</v>
       </c>
       <c r="O73" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P73" s="17">
         <v>1</v>
       </c>
       <c r="Q73" s="17" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="R73" s="17" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="S73" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T73" s="17" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="U73" s="17" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="V73" s="17">
         <v>150</v>
       </c>
       <c r="W73" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X73" s="17">
         <v>1</v>
@@ -12863,30 +12919,30 @@
         <v>54500</v>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="409.5">
+    <row r="74" spans="1:26">
       <c r="A74" s="17">
         <v>63</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G74" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H74" s="17" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I74" s="17">
         <v>11</v>
@@ -12895,43 +12951,43 @@
         <v>21799480376</v>
       </c>
       <c r="K74" s="17" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="M74" s="71" t="s">
-        <v>771</v>
+        <v>670</v>
+      </c>
+      <c r="M74" s="65" t="s">
+        <v>768</v>
       </c>
       <c r="N74" s="17">
         <v>132</v>
       </c>
       <c r="O74" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P74" s="17">
         <v>1</v>
       </c>
       <c r="Q74" s="17" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="R74" s="17" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="S74" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T74" s="17" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="U74" s="17" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="V74" s="17">
         <v>132</v>
       </c>
       <c r="W74" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X74" s="17">
         <v>1</v>
@@ -12943,30 +12999,30 @@
         <v>54500</v>
       </c>
     </row>
-    <row r="75" spans="1:26" ht="409.5">
+    <row r="75" spans="1:26">
       <c r="A75" s="17">
         <v>64</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D75" s="17" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E75" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G75" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H75" s="17" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I75" s="17">
         <v>12</v>
@@ -12975,43 +13031,43 @@
         <v>21800790512</v>
       </c>
       <c r="K75" s="17" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="M75" s="71" t="s">
-        <v>772</v>
+        <v>672</v>
+      </c>
+      <c r="M75" s="65" t="s">
+        <v>769</v>
       </c>
       <c r="N75" s="17">
         <v>112</v>
       </c>
       <c r="O75" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P75" s="17">
         <v>1</v>
       </c>
       <c r="Q75" s="17" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="R75" s="17" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="S75" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T75" s="17" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="U75" s="17" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="V75" s="17">
         <v>112</v>
       </c>
       <c r="W75" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X75" s="17">
         <v>1</v>
@@ -13023,30 +13079,30 @@
         <v>54500</v>
       </c>
     </row>
-    <row r="76" spans="1:26" ht="409.5">
+    <row r="76" spans="1:26">
       <c r="A76" s="17">
         <v>65</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="D76" s="17" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="E76" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G76" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H76" s="17" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I76" s="17">
         <v>13</v>
@@ -13055,43 +13111,43 @@
         <v>21793228443</v>
       </c>
       <c r="K76" s="17" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="M76" s="71" t="s">
-        <v>773</v>
+        <v>674</v>
+      </c>
+      <c r="M76" s="65" t="s">
+        <v>770</v>
       </c>
       <c r="N76" s="17">
         <v>128</v>
       </c>
       <c r="O76" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P76" s="17">
         <v>1</v>
       </c>
       <c r="Q76" s="17" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="R76" s="17" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="S76" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T76" s="17" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="U76" s="17" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="V76" s="17">
         <v>32</v>
       </c>
       <c r="W76" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X76" s="17">
         <v>4</v>
@@ -13103,30 +13159,30 @@
         <v>42900</v>
       </c>
     </row>
-    <row r="77" spans="1:26" ht="409.5">
+    <row r="77" spans="1:26">
       <c r="A77" s="17">
         <v>66</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="E77" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F77" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G77" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I77" s="17">
         <v>14</v>
@@ -13135,43 +13191,43 @@
         <v>21793256416</v>
       </c>
       <c r="K77" s="17" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>679</v>
-      </c>
-      <c r="M77" s="71" t="s">
-        <v>774</v>
+        <v>676</v>
+      </c>
+      <c r="M77" s="65" t="s">
+        <v>771</v>
       </c>
       <c r="N77" s="17">
         <v>116</v>
       </c>
       <c r="O77" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P77" s="17">
         <v>1</v>
       </c>
       <c r="Q77" s="17" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="R77" s="17" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="S77" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T77" s="17" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="U77" s="17" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="V77" s="17">
         <v>29</v>
       </c>
       <c r="W77" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X77" s="17">
         <v>4</v>
@@ -13183,30 +13239,30 @@
         <v>42900</v>
       </c>
     </row>
-    <row r="78" spans="1:26" ht="409.5">
+    <row r="78" spans="1:26">
       <c r="A78" s="17">
         <v>67</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E78" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F78" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G78" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H78" s="17" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I78" s="17">
         <v>15</v>
@@ -13215,43 +13271,43 @@
         <v>21793256419</v>
       </c>
       <c r="K78" s="17" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>681</v>
-      </c>
-      <c r="M78" s="71" t="s">
-        <v>775</v>
+        <v>678</v>
+      </c>
+      <c r="M78" s="65" t="s">
+        <v>772</v>
       </c>
       <c r="N78" s="17">
         <v>104</v>
       </c>
       <c r="O78" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P78" s="17">
         <v>1</v>
       </c>
       <c r="Q78" s="17" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="R78" s="17" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="S78" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T78" s="17" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="U78" s="17" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="V78" s="17">
         <v>26</v>
       </c>
       <c r="W78" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X78" s="17">
         <v>4</v>
@@ -13263,30 +13319,30 @@
         <v>42900</v>
       </c>
     </row>
-    <row r="79" spans="1:26" ht="409.5">
+    <row r="79" spans="1:26">
       <c r="A79" s="17">
         <v>68</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="E79" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F79" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I79" s="17">
         <v>16</v>
@@ -13295,43 +13351,43 @@
         <v>21968910906</v>
       </c>
       <c r="K79" s="17" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="M79" s="71" t="s">
-        <v>776</v>
+        <v>680</v>
+      </c>
+      <c r="M79" s="65" t="s">
+        <v>773</v>
       </c>
       <c r="N79" s="17">
         <v>88</v>
       </c>
       <c r="O79" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P79" s="17">
         <v>1</v>
       </c>
       <c r="Q79" s="17" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="R79" s="17" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="S79" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T79" s="17" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="U79" s="17" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="V79" s="17">
         <v>22</v>
       </c>
       <c r="W79" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X79" s="17">
         <v>4</v>
@@ -13343,30 +13399,30 @@
         <v>42900</v>
       </c>
     </row>
-    <row r="80" spans="1:26" ht="409.5">
+    <row r="80" spans="1:26">
       <c r="A80" s="17">
         <v>69</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="E80" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F80" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G80" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H80" s="17" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I80" s="17">
         <v>17</v>
@@ -13375,43 +13431,43 @@
         <v>21793284456</v>
       </c>
       <c r="K80" s="17" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="M80" s="71" t="s">
-        <v>777</v>
+        <v>682</v>
+      </c>
+      <c r="M80" s="65" t="s">
+        <v>774</v>
       </c>
       <c r="N80" s="17">
         <v>76</v>
       </c>
       <c r="O80" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P80" s="17">
         <v>1</v>
       </c>
       <c r="Q80" s="17" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="R80" s="17" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="S80" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T80" s="17" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="U80" s="17" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="V80" s="17">
         <v>19</v>
       </c>
       <c r="W80" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X80" s="17">
         <v>4</v>
@@ -13423,30 +13479,30 @@
         <v>42900</v>
       </c>
     </row>
-    <row r="81" spans="1:26" ht="409.5">
+    <row r="81" spans="1:26">
       <c r="A81" s="17">
         <v>70</v>
       </c>
       <c r="B81" s="17" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="E81" s="17" t="s">
         <v>153</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G81" s="17" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H81" s="17" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="I81" s="17">
         <v>18</v>
@@ -13455,43 +13511,43 @@
         <v>23399582505</v>
       </c>
       <c r="K81" s="17" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="M81" s="71" t="s">
-        <v>778</v>
+        <v>684</v>
+      </c>
+      <c r="M81" s="65" t="s">
+        <v>775</v>
       </c>
       <c r="N81" s="17">
         <v>64</v>
       </c>
       <c r="O81" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="P81" s="17">
         <v>1</v>
       </c>
       <c r="Q81" s="17" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="R81" s="17" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="S81" s="17" t="s">
         <v>157</v>
       </c>
       <c r="T81" s="17" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="U81" s="17" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="V81" s="17">
         <v>16</v>
       </c>
       <c r="W81" s="17" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="X81" s="17">
         <v>4</v>
@@ -13642,9 +13698,11 @@
     <hyperlink ref="L73" r:id="rId118" xr:uid="{08AA3B0B-5A39-4FE8-A037-B79F1B6732E0}"/>
     <hyperlink ref="L74" r:id="rId119" xr:uid="{A4EEE11E-613B-4673-AB82-B49B140328D5}"/>
     <hyperlink ref="L78" r:id="rId120" xr:uid="{F906F186-5393-4B72-B5FE-EA66A418B024}"/>
+    <hyperlink ref="U39" r:id="rId121" xr:uid="{26E6BED6-4A3F-4395-B762-09DAF12A3D17}"/>
+    <hyperlink ref="U41" r:id="rId122" xr:uid="{5B9D112A-2E91-4AB6-A662-AEFCF04E96B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId121"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId123"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
KeyError due to URL delete
</commit_message>
<xml_diff>
--- a/data/Liberation_Price Tracker SKU list_v1_Pampers.xlsx
+++ b/data/Liberation_Price Tracker SKU list_v1_Pampers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pgone-my.sharepoint.com/personal/kang_y_5_pg_com1/Documents/Documents/GitHub/liberation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{17BCC08E-1F5D-4046-8FCF-30AF4568CA99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{52AFDCC4-1218-4CBF-BD7A-C59473120D2A}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="8_{17BCC08E-1F5D-4046-8FCF-30AF4568CA99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{86FBD2CB-733D-4655-A1F2-5068811FFFC2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="779" xr2:uid="{082D8A25-05B0-4134-80F4-C81249D6F8B7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2100" uniqueCount="785">
   <si>
     <t>No</t>
     <phoneticPr fontId="5"/>
@@ -4885,6 +4885,9 @@
   -H 'Accept-Language: en-US,en;q=0.9' \
   -H 'Cookie: NNB=ADCTWOFKCFPV6; AD_SHP_BID=16; ASID=01ea3946000001752655f0bd0000004d; NID_AUT=ycinsRPvqCHMmoSZytu0APej0V7IwJBJtsU/O7g6h+vc9wAskP25ddE1DZ6vQCX8; NID_JKL=fEgYRAtn7E6D//aEtRcykTjrY/lm4elu/Y7NAGOhHhM=; _ga=GA1.2.1060104753.1603100818; NRTK=ag#20s_gr#1_ma#-2_si#0_en#0_sp#0; MM_NEW=1; NFS=2; MM_NOW_COACH=1; NID_SES=AAABnJRDbhBfyvobBHn7LYxr5Zn8Y2kJOXY2oDhkF3IoN7UW5hPP8DQT4iuqa651AbPPw5lF4Uzh/gSyuUmiXW39nkY7MkaS+0e/7BLwEzuLsP0SaDhDUtDOWj+p2DjRxq87Mm0fKSefD+75wAtMWuofTp5joTO42Vszy10KzONx7MZjUBVn6eq0dz4zh6pnQwm2b2yAidZlweAJGSRKm66OyMAZputPcv3xuO5PSbh/udhHh0FQ4ati1ywTadjytC/Mi/k5EFYxH1bDijby2Au1vC15g1SlCYBQ7HjTDsUUHpwTWVqElJ6pcXENTJesJpOILu+OOo+D1O/XAVXkYdtAg9B1PDMSC8H5lcX2UmMxmtbLuu0NdYoQyzcijpFzQBJrjPA0A3cZrvgy2sHQJNAfBC1Ss+phxrz+t6pkVDJc08PK1rmOea/cj2X9kCaMscak2ylCMSFfyIzbi7+NzufQInHNUxJ569agfaXX43DleU38BWwb+RfDauZyQpuLgchK8rI3nL0Nkuhft0Fmzh2NIl+v9F8BuIbFQQFuD0K+lGus; spage_uid=' \
   --compressed</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/lite.nhn?nvMid=24556793801</t>
   </si>
 </sst>
 </file>
@@ -5380,7 +5383,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5599,6 +5602,9 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="18" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7401,10 +7407,10 @@
   <dimension ref="A1:BJ81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" ySplit="11" topLeftCell="M48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="11" topLeftCell="K15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="M67" sqref="M67"/>
+      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -7556,10 +7562,10 @@
       <c r="X8" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="Y8" s="76" t="s">
+      <c r="Y8" s="77" t="s">
         <v>133</v>
       </c>
-      <c r="Z8" s="76"/>
+      <c r="Z8" s="77"/>
       <c r="AA8" s="8"/>
       <c r="AB8" s="8"/>
       <c r="AC8" s="8"/>
@@ -7615,155 +7621,155 @@
     </row>
     <row r="9" spans="1:62" ht="15.75">
       <c r="A9" s="7"/>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="78"/>
-      <c r="P9" s="78"/>
-      <c r="Q9" s="78"/>
-      <c r="R9" s="78"/>
-      <c r="S9" s="78"/>
-      <c r="T9" s="78"/>
-      <c r="U9" s="78"/>
-      <c r="V9" s="78"/>
-      <c r="W9" s="78"/>
-      <c r="X9" s="78"/>
-      <c r="Y9" s="78"/>
-      <c r="Z9" s="79"/>
-      <c r="AA9" s="80" t="s">
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="79"/>
+      <c r="Q9" s="79"/>
+      <c r="R9" s="79"/>
+      <c r="S9" s="79"/>
+      <c r="T9" s="79"/>
+      <c r="U9" s="79"/>
+      <c r="V9" s="79"/>
+      <c r="W9" s="79"/>
+      <c r="X9" s="79"/>
+      <c r="Y9" s="79"/>
+      <c r="Z9" s="80"/>
+      <c r="AA9" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="AB9" s="81"/>
-      <c r="AC9" s="81"/>
-      <c r="AD9" s="81"/>
-      <c r="AE9" s="81"/>
-      <c r="AF9" s="81"/>
-      <c r="AG9" s="81"/>
-      <c r="AH9" s="81"/>
-      <c r="AI9" s="81"/>
-      <c r="AJ9" s="81"/>
-      <c r="AK9" s="81"/>
-      <c r="AL9" s="81"/>
-      <c r="AM9" s="81"/>
-      <c r="AN9" s="81"/>
-      <c r="AO9" s="81"/>
-      <c r="AP9" s="81"/>
-      <c r="AQ9" s="81"/>
-      <c r="AR9" s="82"/>
-      <c r="AS9" s="83" t="s">
+      <c r="AB9" s="82"/>
+      <c r="AC9" s="82"/>
+      <c r="AD9" s="82"/>
+      <c r="AE9" s="82"/>
+      <c r="AF9" s="82"/>
+      <c r="AG9" s="82"/>
+      <c r="AH9" s="82"/>
+      <c r="AI9" s="82"/>
+      <c r="AJ9" s="82"/>
+      <c r="AK9" s="82"/>
+      <c r="AL9" s="82"/>
+      <c r="AM9" s="82"/>
+      <c r="AN9" s="82"/>
+      <c r="AO9" s="82"/>
+      <c r="AP9" s="82"/>
+      <c r="AQ9" s="82"/>
+      <c r="AR9" s="83"/>
+      <c r="AS9" s="84" t="s">
         <v>135</v>
       </c>
-      <c r="AT9" s="84"/>
-      <c r="AU9" s="84"/>
-      <c r="AV9" s="84"/>
-      <c r="AW9" s="84"/>
-      <c r="AX9" s="84"/>
-      <c r="AY9" s="84"/>
-      <c r="AZ9" s="84"/>
-      <c r="BA9" s="84"/>
-      <c r="BB9" s="84"/>
-      <c r="BC9" s="84"/>
-      <c r="BD9" s="84"/>
-      <c r="BE9" s="84"/>
-      <c r="BF9" s="84"/>
-      <c r="BG9" s="84"/>
-      <c r="BH9" s="84"/>
-      <c r="BI9" s="84"/>
-      <c r="BJ9" s="85"/>
+      <c r="AT9" s="85"/>
+      <c r="AU9" s="85"/>
+      <c r="AV9" s="85"/>
+      <c r="AW9" s="85"/>
+      <c r="AX9" s="85"/>
+      <c r="AY9" s="85"/>
+      <c r="AZ9" s="85"/>
+      <c r="BA9" s="85"/>
+      <c r="BB9" s="85"/>
+      <c r="BC9" s="85"/>
+      <c r="BD9" s="85"/>
+      <c r="BE9" s="85"/>
+      <c r="BF9" s="85"/>
+      <c r="BG9" s="85"/>
+      <c r="BH9" s="85"/>
+      <c r="BI9" s="85"/>
+      <c r="BJ9" s="86"/>
     </row>
     <row r="10" spans="1:62">
       <c r="A10" s="4"/>
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="87" t="s">
         <v>314</v>
       </c>
-      <c r="C10" s="87"/>
-      <c r="D10" s="87"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="87"/>
-      <c r="H10" s="87"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="74" t="s">
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="74"/>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="75" t="s">
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="75"/>
+      <c r="O10" s="75"/>
+      <c r="P10" s="75"/>
+      <c r="Q10" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="R10" s="75"/>
-      <c r="S10" s="75"/>
-      <c r="T10" s="75"/>
-      <c r="U10" s="75"/>
-      <c r="V10" s="75"/>
-      <c r="W10" s="75"/>
-      <c r="X10" s="75"/>
-      <c r="Y10" s="75"/>
-      <c r="Z10" s="75"/>
-      <c r="AA10" s="73" t="s">
+      <c r="R10" s="76"/>
+      <c r="S10" s="76"/>
+      <c r="T10" s="76"/>
+      <c r="U10" s="76"/>
+      <c r="V10" s="76"/>
+      <c r="W10" s="76"/>
+      <c r="X10" s="76"/>
+      <c r="Y10" s="76"/>
+      <c r="Z10" s="76"/>
+      <c r="AA10" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="AB10" s="73"/>
-      <c r="AC10" s="73"/>
-      <c r="AD10" s="73"/>
-      <c r="AE10" s="73"/>
-      <c r="AF10" s="74" t="s">
+      <c r="AB10" s="74"/>
+      <c r="AC10" s="74"/>
+      <c r="AD10" s="74"/>
+      <c r="AE10" s="74"/>
+      <c r="AF10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="AG10" s="74"/>
-      <c r="AH10" s="74"/>
-      <c r="AI10" s="74"/>
-      <c r="AJ10" s="74"/>
-      <c r="AK10" s="74"/>
-      <c r="AL10" s="75" t="s">
+      <c r="AG10" s="75"/>
+      <c r="AH10" s="75"/>
+      <c r="AI10" s="75"/>
+      <c r="AJ10" s="75"/>
+      <c r="AK10" s="75"/>
+      <c r="AL10" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="AM10" s="75"/>
-      <c r="AN10" s="75"/>
-      <c r="AO10" s="75"/>
-      <c r="AP10" s="75"/>
-      <c r="AQ10" s="75"/>
-      <c r="AR10" s="75"/>
-      <c r="AS10" s="73" t="s">
+      <c r="AM10" s="76"/>
+      <c r="AN10" s="76"/>
+      <c r="AO10" s="76"/>
+      <c r="AP10" s="76"/>
+      <c r="AQ10" s="76"/>
+      <c r="AR10" s="76"/>
+      <c r="AS10" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="AT10" s="73"/>
-      <c r="AU10" s="73"/>
-      <c r="AV10" s="73"/>
-      <c r="AW10" s="73"/>
-      <c r="AX10" s="74" t="s">
+      <c r="AT10" s="74"/>
+      <c r="AU10" s="74"/>
+      <c r="AV10" s="74"/>
+      <c r="AW10" s="74"/>
+      <c r="AX10" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="AY10" s="74"/>
-      <c r="AZ10" s="74"/>
-      <c r="BA10" s="74"/>
-      <c r="BB10" s="74"/>
-      <c r="BC10" s="74"/>
-      <c r="BD10" s="75" t="s">
+      <c r="AY10" s="75"/>
+      <c r="AZ10" s="75"/>
+      <c r="BA10" s="75"/>
+      <c r="BB10" s="75"/>
+      <c r="BC10" s="75"/>
+      <c r="BD10" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="BE10" s="75"/>
-      <c r="BF10" s="75"/>
-      <c r="BG10" s="75"/>
-      <c r="BH10" s="75"/>
-      <c r="BI10" s="75"/>
-      <c r="BJ10" s="75"/>
+      <c r="BE10" s="76"/>
+      <c r="BF10" s="76"/>
+      <c r="BG10" s="76"/>
+      <c r="BH10" s="76"/>
+      <c r="BI10" s="76"/>
+      <c r="BJ10" s="76"/>
     </row>
     <row r="11" spans="1:62">
       <c r="A11" s="10" t="s">
@@ -8297,7 +8303,7 @@
       <c r="K16" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="L16" s="35" t="s">
+      <c r="L16" s="73" t="s">
         <v>166</v>
       </c>
       <c r="M16" s="71" t="s">
@@ -9392,7 +9398,7 @@
       <c r="K30" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="L30" s="35" t="s">
+      <c r="L30" s="73" t="s">
         <v>218</v>
       </c>
       <c r="M30" s="72"/>
@@ -9470,8 +9476,8 @@
       <c r="K31" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="L31" s="35" t="s">
-        <v>222</v>
+      <c r="L31" s="73" t="s">
+        <v>784</v>
       </c>
       <c r="M31" s="71"/>
       <c r="N31" s="16">
@@ -13598,108 +13604,108 @@
     <hyperlink ref="L28" r:id="rId18" xr:uid="{BAFF46B9-E283-4748-8680-34B6C456DD40}"/>
     <hyperlink ref="L29" r:id="rId19" xr:uid="{40F5B568-1AD1-4D27-8B5C-6E7976F384E0}"/>
     <hyperlink ref="L30" r:id="rId20" xr:uid="{60F19C97-460E-4EA3-BCC5-786BD138C16C}"/>
-    <hyperlink ref="L31" r:id="rId21" xr:uid="{22FEB9A6-CA72-443D-86AB-F6BBCE041DCC}"/>
-    <hyperlink ref="U14" r:id="rId22" display="https://www.coupang.com/vp/products/324202666?itemId=1038077454" xr:uid="{04F03823-D2FB-4E15-8001-E81DFAC12C7E}"/>
-    <hyperlink ref="U15" r:id="rId23" display="https://www.coupang.com/vp/products/324202651?itemId=1038077401" xr:uid="{1090DAFD-91E5-4AFD-8205-0BA4966EE585}"/>
-    <hyperlink ref="U17" r:id="rId24" display="https://www.coupang.com/vp/products/1370801527?itemId=2403399112" xr:uid="{1B9A937B-FCD7-4D5F-8EDD-558F7B62E57F}"/>
-    <hyperlink ref="U18" r:id="rId25" display="https://www.coupang.com/vp/products/127467695?itemId=877623215" xr:uid="{EF9A4D17-AD81-4B02-82F4-719935E0DB1C}"/>
-    <hyperlink ref="U16" r:id="rId26" xr:uid="{9AB4EA10-60B9-42F6-AF30-9FA4971B8868}"/>
-    <hyperlink ref="U20" r:id="rId27" display="https://www.coupang.com/vp/products/5740084?itemId=6751262" xr:uid="{D8B986E9-F158-4D75-BDE1-4AB0F37546B3}"/>
-    <hyperlink ref="U21" r:id="rId28" xr:uid="{03B58A62-F929-4A77-80F3-7ECB0CCECE80}"/>
-    <hyperlink ref="U22" r:id="rId29" xr:uid="{E6D3DEFE-9733-44FC-9FB5-E51AD1D10CEB}"/>
-    <hyperlink ref="U23" r:id="rId30" xr:uid="{4CE251AF-AC3D-45CC-A837-D94A8ABF9C86}"/>
-    <hyperlink ref="U24" r:id="rId31" xr:uid="{B6BF95CD-24A0-4BB6-858B-15771DB59305}"/>
-    <hyperlink ref="U25" r:id="rId32" xr:uid="{97CA5A5B-F17F-4020-9EAE-2CF31E77BB28}"/>
-    <hyperlink ref="U26" r:id="rId33" xr:uid="{1CB70BC6-FCFD-4C26-8511-8FEA26790711}"/>
-    <hyperlink ref="U27" r:id="rId34" xr:uid="{C969AE79-5A82-4E64-B3E7-4C46690B7875}"/>
-    <hyperlink ref="U28" r:id="rId35" xr:uid="{8D2683ED-9A30-4C13-81E6-64B591295759}"/>
-    <hyperlink ref="U29" r:id="rId36" xr:uid="{74B9F7B1-C76B-4864-8EBC-A9F0DE801400}"/>
-    <hyperlink ref="U30" r:id="rId37" xr:uid="{60A89D4A-4939-477E-B10C-9E313DE6160C}"/>
-    <hyperlink ref="U31" r:id="rId38" xr:uid="{EA677EA9-7F85-4855-9ED4-7B34F8FAB7CD}"/>
-    <hyperlink ref="U19" r:id="rId39" xr:uid="{8FDB9BD7-5CFF-476B-BBF5-5633F058AE6D}"/>
-    <hyperlink ref="L45" r:id="rId40" xr:uid="{B17DF844-77F9-43AB-ADEC-7E8C7C10AD79}"/>
-    <hyperlink ref="L46" r:id="rId41" xr:uid="{6234E9B6-3983-4783-BEF0-AC55188F6BA8}"/>
-    <hyperlink ref="L47" r:id="rId42" xr:uid="{CA8D0F46-CB1F-405E-B3E7-FB46CB1F330D}"/>
-    <hyperlink ref="L48" r:id="rId43" xr:uid="{22A2824E-88EE-41D1-82DC-19934AB64B4B}"/>
-    <hyperlink ref="L52" r:id="rId44" xr:uid="{81E3EE2F-E27C-4CD6-A61E-29E9F51021A8}"/>
-    <hyperlink ref="L53" r:id="rId45" xr:uid="{ED1D2281-ADF8-4E61-87D2-A3C1DADC46C3}"/>
-    <hyperlink ref="L55" r:id="rId46" xr:uid="{35FE9C18-0617-410E-A295-7F0C37B79789}"/>
-    <hyperlink ref="L54" r:id="rId47" xr:uid="{55AF23FC-2731-43D6-9BFC-E5B3FB6A6AC9}"/>
-    <hyperlink ref="L49" r:id="rId48" xr:uid="{C5630D55-397A-4777-8669-39F1119480DF}"/>
-    <hyperlink ref="U46" r:id="rId49" xr:uid="{FD98A686-828A-45C9-892F-CABACB07DBD1}"/>
-    <hyperlink ref="U47" r:id="rId50" xr:uid="{D69BD7AF-A395-4884-9C0C-458297D43D58}"/>
-    <hyperlink ref="U48" r:id="rId51" xr:uid="{8259D4D9-B317-4856-9144-A93652990C73}"/>
-    <hyperlink ref="U53" r:id="rId52" display="https://www.coupang.com/vp/products/3199234?itemId=3903076" xr:uid="{0CE981E0-C1C2-45B8-9660-8BAE99D4B241}"/>
-    <hyperlink ref="U55" r:id="rId53" xr:uid="{D6EDB869-4EBD-47F4-A90B-CB15FD6A6F54}"/>
-    <hyperlink ref="U54" r:id="rId54" xr:uid="{BC5F4EFF-0F80-4BFB-BEC9-6AD383AC4832}"/>
-    <hyperlink ref="L32" r:id="rId55" xr:uid="{62B4498E-19AA-4F57-AE4F-BBE676775ADC}"/>
-    <hyperlink ref="L33" r:id="rId56" xr:uid="{D756429B-99DB-4773-9E25-58A58F392496}"/>
-    <hyperlink ref="L34" r:id="rId57" xr:uid="{F595FE2E-4915-47DD-A0D5-8C968145FDD6}"/>
-    <hyperlink ref="L35" r:id="rId58" xr:uid="{56D7279D-CB13-410F-A869-AAFC80964A80}"/>
-    <hyperlink ref="L36" r:id="rId59" xr:uid="{6483CDDF-8A85-44DE-8115-60B39A9671E7}"/>
-    <hyperlink ref="L37" r:id="rId60" xr:uid="{67375352-BD5B-420A-9526-521CB97448D7}"/>
-    <hyperlink ref="L38" r:id="rId61" xr:uid="{24BC91B0-F7B9-49EE-9BEF-BA5EEB94B730}"/>
-    <hyperlink ref="L39" r:id="rId62" xr:uid="{AED6501B-2ED5-4A7E-B8E7-379B19482ABF}"/>
-    <hyperlink ref="L40" r:id="rId63" xr:uid="{DBC798BB-8111-48E3-A9BB-634A4FB1DDBB}"/>
-    <hyperlink ref="L43" r:id="rId64" xr:uid="{D1BD140C-8A4B-4636-83A3-ACD9B3A91CCC}"/>
-    <hyperlink ref="L42" r:id="rId65" xr:uid="{A5AC2415-FA59-440E-9799-4BAE4D8ECF69}"/>
-    <hyperlink ref="L41" r:id="rId66" xr:uid="{3E9EF113-69B5-4355-9559-8B77D01C44C0}"/>
-    <hyperlink ref="U32" r:id="rId67" xr:uid="{2875B798-23FA-49D9-B917-614117374100}"/>
-    <hyperlink ref="U33" r:id="rId68" xr:uid="{681E1C93-6AA2-4072-A6F4-40653AC37A1E}"/>
-    <hyperlink ref="U34" r:id="rId69" xr:uid="{5DC29752-4B0A-4A99-8F8C-C018F7AE50B5}"/>
-    <hyperlink ref="U35" r:id="rId70" xr:uid="{E7A777CE-0C12-4853-8E0E-70BC79483B66}"/>
-    <hyperlink ref="U36" r:id="rId71" xr:uid="{2421B3DD-D036-4901-B622-4154C44C2021}"/>
-    <hyperlink ref="U37" r:id="rId72" xr:uid="{D70307DD-A493-472A-9EC1-D8D6E9A6C781}"/>
-    <hyperlink ref="U44" r:id="rId73" xr:uid="{43852961-DB7B-46A4-BA1A-A522C9DF7535}"/>
-    <hyperlink ref="U38" r:id="rId74" xr:uid="{76429066-FC34-4BDB-8141-A45F5EAFE08B}"/>
-    <hyperlink ref="U42" r:id="rId75" xr:uid="{9074EB9D-C024-44FD-8EA1-95D1BB70AC70}"/>
-    <hyperlink ref="U43" r:id="rId76" xr:uid="{A8615043-71A4-476B-A537-90911A2A5ADB}"/>
-    <hyperlink ref="L18" r:id="rId77" xr:uid="{543194B7-6C66-48F0-AF88-784789160F0E}"/>
-    <hyperlink ref="U40" r:id="rId78" xr:uid="{2E85DA23-C86C-4F67-96B4-9B8444B74431}"/>
-    <hyperlink ref="U45" r:id="rId79" display="https://www.coupang.com/vp/products/24131490?itemId=93945069&amp;vendorItemId=3000229112&amp;pickType=COU_PICK&amp;q=%EC%98%A4%EB%9E%84%EB%B9%84+%EB%AF%BC%ED%8A%B8cltlf&amp;itemsCount=36&amp;searchId=2665333e226945279bfd03f1c92698b2&amp;rank=1&amp;isAddedCart=" xr:uid="{8878FB12-0034-4FD8-A435-7E06109BFEC4}"/>
-    <hyperlink ref="U49" r:id="rId80" xr:uid="{EABEE546-F84D-4292-8C2E-B33C4877732D}"/>
-    <hyperlink ref="L51" r:id="rId81" xr:uid="{AB730EBC-7FDD-4820-A78B-456F728B1349}"/>
-    <hyperlink ref="U52" r:id="rId82" xr:uid="{C924ABF8-D7E5-437B-BE3F-3199ED07ECFC}"/>
-    <hyperlink ref="U51" r:id="rId83" xr:uid="{589BBE6D-14FD-4C0D-86AF-F333E9E4737C}"/>
-    <hyperlink ref="U50" r:id="rId84" xr:uid="{27E84478-EACD-4CBF-AE0D-B504709F7ECE}"/>
-    <hyperlink ref="L50" r:id="rId85" xr:uid="{75180D2D-565D-408F-8CF4-B569054DCA4D}"/>
-    <hyperlink ref="L44" r:id="rId86" xr:uid="{10CA2363-69ED-46B0-940F-0B27ACEC1050}"/>
-    <hyperlink ref="U57" r:id="rId87" xr:uid="{9B9CEA7E-A8C0-42FD-A7DF-10BAE5FF64D2}"/>
-    <hyperlink ref="U60" r:id="rId88" xr:uid="{62BB41C8-CA59-48C6-A6C6-477ECD049E03}"/>
-    <hyperlink ref="U58" r:id="rId89" xr:uid="{8993D2F1-A0D0-4C8E-9963-C130621A3DBD}"/>
-    <hyperlink ref="U63" r:id="rId90" xr:uid="{EFCBA801-359B-4A89-BB1E-BE28595A399E}"/>
-    <hyperlink ref="U61" r:id="rId91" xr:uid="{A772F0B6-53B4-40C9-A5FE-749EB2B6480C}"/>
-    <hyperlink ref="L57" r:id="rId92" xr:uid="{CEA7C2E8-7FFA-4494-B2E4-FD03AB68ACA4}"/>
-    <hyperlink ref="L59" r:id="rId93" xr:uid="{D7C9A5A3-92D7-4181-8458-4B18B07BC69A}"/>
-    <hyperlink ref="L60" r:id="rId94" xr:uid="{E5EB2A0A-5CC9-45ED-BBB9-929ABFCD6FFC}"/>
-    <hyperlink ref="L63" r:id="rId95" xr:uid="{C8BBE869-F0F8-4B2D-9093-63398AFDB30B}"/>
-    <hyperlink ref="L62" r:id="rId96" xr:uid="{2A2AF402-E871-4AA1-9682-F8052E3D81EA}"/>
-    <hyperlink ref="L61" r:id="rId97" xr:uid="{73884DE0-87AB-495B-B3A3-E8A2BE4DE099}"/>
-    <hyperlink ref="L58" r:id="rId98" xr:uid="{9FAEF5AD-233F-41A9-A3C2-87A8B5C0F0A9}"/>
-    <hyperlink ref="L56" r:id="rId99" xr:uid="{50EF3DC3-6799-43AD-985E-9115AC929ED6}"/>
-    <hyperlink ref="U56" r:id="rId100" xr:uid="{80E1C5AE-18D7-413E-B4EB-5DCDAAA83642}"/>
-    <hyperlink ref="U59" r:id="rId101" xr:uid="{12412E87-36B6-4B71-8F66-00F618ED0BF9}"/>
-    <hyperlink ref="U62" r:id="rId102" xr:uid="{19052DF1-50DA-45C0-AA8D-DF545EBFD0B7}"/>
-    <hyperlink ref="L64" r:id="rId103" xr:uid="{A6972B9A-11EC-4505-BB9C-2E43F0FB1359}"/>
-    <hyperlink ref="L65" r:id="rId104" xr:uid="{26C63059-8E84-45D7-92A6-860CD6933B7B}"/>
-    <hyperlink ref="L67" r:id="rId105" xr:uid="{F89BE908-746E-4EF7-ADB9-49BB99BFE045}"/>
-    <hyperlink ref="L69" r:id="rId106" xr:uid="{3810B59D-3C20-466F-9A30-0ADA576C9A23}"/>
-    <hyperlink ref="L71" r:id="rId107" xr:uid="{EB4C92E4-1242-4D64-91DF-0DE2E13E68FB}"/>
-    <hyperlink ref="L72" r:id="rId108" xr:uid="{2436ACB7-8CBE-4404-AB5D-6B4C22D775C3}"/>
-    <hyperlink ref="L75" r:id="rId109" xr:uid="{C4B27291-6EF3-4D11-8E80-4D291A6D89B6}"/>
-    <hyperlink ref="L76" r:id="rId110" xr:uid="{CE0B7581-A52B-4160-8992-25B0C5808961}"/>
-    <hyperlink ref="L77" r:id="rId111" xr:uid="{16AD970A-FACC-44EC-A1DA-25531A342731}"/>
-    <hyperlink ref="L79" r:id="rId112" xr:uid="{9D4B6EC4-19CB-4557-BE79-4136A2324550}"/>
-    <hyperlink ref="L80" r:id="rId113" xr:uid="{1A9BCA50-BE0C-4B22-A957-3B80712A2B17}"/>
-    <hyperlink ref="L81" r:id="rId114" xr:uid="{0DF291A6-D086-4CE4-B085-B94C715854AF}"/>
-    <hyperlink ref="L66" r:id="rId115" xr:uid="{868B7E99-AED5-4C00-8167-874AFB651830}"/>
-    <hyperlink ref="L68" r:id="rId116" xr:uid="{473DD8F3-5261-4CEC-A852-6CC3118CDF7E}"/>
-    <hyperlink ref="L70" r:id="rId117" xr:uid="{B4DA8F59-E30F-47C5-A54E-C36D8538B462}"/>
-    <hyperlink ref="L73" r:id="rId118" xr:uid="{08AA3B0B-5A39-4FE8-A037-B79F1B6732E0}"/>
-    <hyperlink ref="L74" r:id="rId119" xr:uid="{A4EEE11E-613B-4673-AB82-B49B140328D5}"/>
-    <hyperlink ref="L78" r:id="rId120" xr:uid="{F906F186-5393-4B72-B5FE-EA66A418B024}"/>
-    <hyperlink ref="U39" r:id="rId121" xr:uid="{26E6BED6-4A3F-4395-B762-09DAF12A3D17}"/>
-    <hyperlink ref="U41" r:id="rId122" xr:uid="{5B9D112A-2E91-4AB6-A662-AEFCF04E96B3}"/>
+    <hyperlink ref="U14" r:id="rId21" display="https://www.coupang.com/vp/products/324202666?itemId=1038077454" xr:uid="{04F03823-D2FB-4E15-8001-E81DFAC12C7E}"/>
+    <hyperlink ref="U15" r:id="rId22" display="https://www.coupang.com/vp/products/324202651?itemId=1038077401" xr:uid="{1090DAFD-91E5-4AFD-8205-0BA4966EE585}"/>
+    <hyperlink ref="U17" r:id="rId23" display="https://www.coupang.com/vp/products/1370801527?itemId=2403399112" xr:uid="{1B9A937B-FCD7-4D5F-8EDD-558F7B62E57F}"/>
+    <hyperlink ref="U18" r:id="rId24" display="https://www.coupang.com/vp/products/127467695?itemId=877623215" xr:uid="{EF9A4D17-AD81-4B02-82F4-719935E0DB1C}"/>
+    <hyperlink ref="U16" r:id="rId25" xr:uid="{9AB4EA10-60B9-42F6-AF30-9FA4971B8868}"/>
+    <hyperlink ref="U20" r:id="rId26" display="https://www.coupang.com/vp/products/5740084?itemId=6751262" xr:uid="{D8B986E9-F158-4D75-BDE1-4AB0F37546B3}"/>
+    <hyperlink ref="U21" r:id="rId27" xr:uid="{03B58A62-F929-4A77-80F3-7ECB0CCECE80}"/>
+    <hyperlink ref="U22" r:id="rId28" xr:uid="{E6D3DEFE-9733-44FC-9FB5-E51AD1D10CEB}"/>
+    <hyperlink ref="U23" r:id="rId29" xr:uid="{4CE251AF-AC3D-45CC-A837-D94A8ABF9C86}"/>
+    <hyperlink ref="U24" r:id="rId30" xr:uid="{B6BF95CD-24A0-4BB6-858B-15771DB59305}"/>
+    <hyperlink ref="U25" r:id="rId31" xr:uid="{97CA5A5B-F17F-4020-9EAE-2CF31E77BB28}"/>
+    <hyperlink ref="U26" r:id="rId32" xr:uid="{1CB70BC6-FCFD-4C26-8511-8FEA26790711}"/>
+    <hyperlink ref="U27" r:id="rId33" xr:uid="{C969AE79-5A82-4E64-B3E7-4C46690B7875}"/>
+    <hyperlink ref="U28" r:id="rId34" xr:uid="{8D2683ED-9A30-4C13-81E6-64B591295759}"/>
+    <hyperlink ref="U29" r:id="rId35" xr:uid="{74B9F7B1-C76B-4864-8EBC-A9F0DE801400}"/>
+    <hyperlink ref="U30" r:id="rId36" xr:uid="{60A89D4A-4939-477E-B10C-9E313DE6160C}"/>
+    <hyperlink ref="U31" r:id="rId37" xr:uid="{EA677EA9-7F85-4855-9ED4-7B34F8FAB7CD}"/>
+    <hyperlink ref="U19" r:id="rId38" xr:uid="{8FDB9BD7-5CFF-476B-BBF5-5633F058AE6D}"/>
+    <hyperlink ref="L45" r:id="rId39" xr:uid="{B17DF844-77F9-43AB-ADEC-7E8C7C10AD79}"/>
+    <hyperlink ref="L46" r:id="rId40" xr:uid="{6234E9B6-3983-4783-BEF0-AC55188F6BA8}"/>
+    <hyperlink ref="L47" r:id="rId41" xr:uid="{CA8D0F46-CB1F-405E-B3E7-FB46CB1F330D}"/>
+    <hyperlink ref="L48" r:id="rId42" xr:uid="{22A2824E-88EE-41D1-82DC-19934AB64B4B}"/>
+    <hyperlink ref="L52" r:id="rId43" xr:uid="{81E3EE2F-E27C-4CD6-A61E-29E9F51021A8}"/>
+    <hyperlink ref="L53" r:id="rId44" xr:uid="{ED1D2281-ADF8-4E61-87D2-A3C1DADC46C3}"/>
+    <hyperlink ref="L55" r:id="rId45" xr:uid="{35FE9C18-0617-410E-A295-7F0C37B79789}"/>
+    <hyperlink ref="L54" r:id="rId46" xr:uid="{55AF23FC-2731-43D6-9BFC-E5B3FB6A6AC9}"/>
+    <hyperlink ref="L49" r:id="rId47" xr:uid="{C5630D55-397A-4777-8669-39F1119480DF}"/>
+    <hyperlink ref="U46" r:id="rId48" xr:uid="{FD98A686-828A-45C9-892F-CABACB07DBD1}"/>
+    <hyperlink ref="U47" r:id="rId49" xr:uid="{D69BD7AF-A395-4884-9C0C-458297D43D58}"/>
+    <hyperlink ref="U48" r:id="rId50" xr:uid="{8259D4D9-B317-4856-9144-A93652990C73}"/>
+    <hyperlink ref="U53" r:id="rId51" display="https://www.coupang.com/vp/products/3199234?itemId=3903076" xr:uid="{0CE981E0-C1C2-45B8-9660-8BAE99D4B241}"/>
+    <hyperlink ref="U55" r:id="rId52" xr:uid="{D6EDB869-4EBD-47F4-A90B-CB15FD6A6F54}"/>
+    <hyperlink ref="U54" r:id="rId53" xr:uid="{BC5F4EFF-0F80-4BFB-BEC9-6AD383AC4832}"/>
+    <hyperlink ref="L32" r:id="rId54" xr:uid="{62B4498E-19AA-4F57-AE4F-BBE676775ADC}"/>
+    <hyperlink ref="L33" r:id="rId55" xr:uid="{D756429B-99DB-4773-9E25-58A58F392496}"/>
+    <hyperlink ref="L34" r:id="rId56" xr:uid="{F595FE2E-4915-47DD-A0D5-8C968145FDD6}"/>
+    <hyperlink ref="L35" r:id="rId57" xr:uid="{56D7279D-CB13-410F-A869-AAFC80964A80}"/>
+    <hyperlink ref="L36" r:id="rId58" xr:uid="{6483CDDF-8A85-44DE-8115-60B39A9671E7}"/>
+    <hyperlink ref="L37" r:id="rId59" xr:uid="{67375352-BD5B-420A-9526-521CB97448D7}"/>
+    <hyperlink ref="L38" r:id="rId60" xr:uid="{24BC91B0-F7B9-49EE-9BEF-BA5EEB94B730}"/>
+    <hyperlink ref="L39" r:id="rId61" xr:uid="{AED6501B-2ED5-4A7E-B8E7-379B19482ABF}"/>
+    <hyperlink ref="L40" r:id="rId62" xr:uid="{DBC798BB-8111-48E3-A9BB-634A4FB1DDBB}"/>
+    <hyperlink ref="L43" r:id="rId63" xr:uid="{D1BD140C-8A4B-4636-83A3-ACD9B3A91CCC}"/>
+    <hyperlink ref="L42" r:id="rId64" xr:uid="{A5AC2415-FA59-440E-9799-4BAE4D8ECF69}"/>
+    <hyperlink ref="L41" r:id="rId65" xr:uid="{3E9EF113-69B5-4355-9559-8B77D01C44C0}"/>
+    <hyperlink ref="U32" r:id="rId66" xr:uid="{2875B798-23FA-49D9-B917-614117374100}"/>
+    <hyperlink ref="U33" r:id="rId67" xr:uid="{681E1C93-6AA2-4072-A6F4-40653AC37A1E}"/>
+    <hyperlink ref="U34" r:id="rId68" xr:uid="{5DC29752-4B0A-4A99-8F8C-C018F7AE50B5}"/>
+    <hyperlink ref="U35" r:id="rId69" xr:uid="{E7A777CE-0C12-4853-8E0E-70BC79483B66}"/>
+    <hyperlink ref="U36" r:id="rId70" xr:uid="{2421B3DD-D036-4901-B622-4154C44C2021}"/>
+    <hyperlink ref="U37" r:id="rId71" xr:uid="{D70307DD-A493-472A-9EC1-D8D6E9A6C781}"/>
+    <hyperlink ref="U44" r:id="rId72" xr:uid="{43852961-DB7B-46A4-BA1A-A522C9DF7535}"/>
+    <hyperlink ref="U38" r:id="rId73" xr:uid="{76429066-FC34-4BDB-8141-A45F5EAFE08B}"/>
+    <hyperlink ref="U42" r:id="rId74" xr:uid="{9074EB9D-C024-44FD-8EA1-95D1BB70AC70}"/>
+    <hyperlink ref="U43" r:id="rId75" xr:uid="{A8615043-71A4-476B-A537-90911A2A5ADB}"/>
+    <hyperlink ref="L18" r:id="rId76" xr:uid="{543194B7-6C66-48F0-AF88-784789160F0E}"/>
+    <hyperlink ref="U40" r:id="rId77" xr:uid="{2E85DA23-C86C-4F67-96B4-9B8444B74431}"/>
+    <hyperlink ref="U45" r:id="rId78" display="https://www.coupang.com/vp/products/24131490?itemId=93945069&amp;vendorItemId=3000229112&amp;pickType=COU_PICK&amp;q=%EC%98%A4%EB%9E%84%EB%B9%84+%EB%AF%BC%ED%8A%B8cltlf&amp;itemsCount=36&amp;searchId=2665333e226945279bfd03f1c92698b2&amp;rank=1&amp;isAddedCart=" xr:uid="{8878FB12-0034-4FD8-A435-7E06109BFEC4}"/>
+    <hyperlink ref="U49" r:id="rId79" xr:uid="{EABEE546-F84D-4292-8C2E-B33C4877732D}"/>
+    <hyperlink ref="L51" r:id="rId80" xr:uid="{AB730EBC-7FDD-4820-A78B-456F728B1349}"/>
+    <hyperlink ref="U52" r:id="rId81" xr:uid="{C924ABF8-D7E5-437B-BE3F-3199ED07ECFC}"/>
+    <hyperlink ref="U51" r:id="rId82" xr:uid="{589BBE6D-14FD-4C0D-86AF-F333E9E4737C}"/>
+    <hyperlink ref="U50" r:id="rId83" xr:uid="{27E84478-EACD-4CBF-AE0D-B504709F7ECE}"/>
+    <hyperlink ref="L50" r:id="rId84" xr:uid="{75180D2D-565D-408F-8CF4-B569054DCA4D}"/>
+    <hyperlink ref="L44" r:id="rId85" xr:uid="{10CA2363-69ED-46B0-940F-0B27ACEC1050}"/>
+    <hyperlink ref="U57" r:id="rId86" xr:uid="{9B9CEA7E-A8C0-42FD-A7DF-10BAE5FF64D2}"/>
+    <hyperlink ref="U60" r:id="rId87" xr:uid="{62BB41C8-CA59-48C6-A6C6-477ECD049E03}"/>
+    <hyperlink ref="U58" r:id="rId88" xr:uid="{8993D2F1-A0D0-4C8E-9963-C130621A3DBD}"/>
+    <hyperlink ref="U63" r:id="rId89" xr:uid="{EFCBA801-359B-4A89-BB1E-BE28595A399E}"/>
+    <hyperlink ref="U61" r:id="rId90" xr:uid="{A772F0B6-53B4-40C9-A5FE-749EB2B6480C}"/>
+    <hyperlink ref="L57" r:id="rId91" xr:uid="{CEA7C2E8-7FFA-4494-B2E4-FD03AB68ACA4}"/>
+    <hyperlink ref="L59" r:id="rId92" xr:uid="{D7C9A5A3-92D7-4181-8458-4B18B07BC69A}"/>
+    <hyperlink ref="L60" r:id="rId93" xr:uid="{E5EB2A0A-5CC9-45ED-BBB9-929ABFCD6FFC}"/>
+    <hyperlink ref="L63" r:id="rId94" xr:uid="{C8BBE869-F0F8-4B2D-9093-63398AFDB30B}"/>
+    <hyperlink ref="L62" r:id="rId95" xr:uid="{2A2AF402-E871-4AA1-9682-F8052E3D81EA}"/>
+    <hyperlink ref="L61" r:id="rId96" xr:uid="{73884DE0-87AB-495B-B3A3-E8A2BE4DE099}"/>
+    <hyperlink ref="L58" r:id="rId97" xr:uid="{9FAEF5AD-233F-41A9-A3C2-87A8B5C0F0A9}"/>
+    <hyperlink ref="L56" r:id="rId98" xr:uid="{50EF3DC3-6799-43AD-985E-9115AC929ED6}"/>
+    <hyperlink ref="U56" r:id="rId99" xr:uid="{80E1C5AE-18D7-413E-B4EB-5DCDAAA83642}"/>
+    <hyperlink ref="U59" r:id="rId100" xr:uid="{12412E87-36B6-4B71-8F66-00F618ED0BF9}"/>
+    <hyperlink ref="U62" r:id="rId101" xr:uid="{19052DF1-50DA-45C0-AA8D-DF545EBFD0B7}"/>
+    <hyperlink ref="L64" r:id="rId102" xr:uid="{A6972B9A-11EC-4505-BB9C-2E43F0FB1359}"/>
+    <hyperlink ref="L65" r:id="rId103" xr:uid="{26C63059-8E84-45D7-92A6-860CD6933B7B}"/>
+    <hyperlink ref="L67" r:id="rId104" xr:uid="{F89BE908-746E-4EF7-ADB9-49BB99BFE045}"/>
+    <hyperlink ref="L69" r:id="rId105" xr:uid="{3810B59D-3C20-466F-9A30-0ADA576C9A23}"/>
+    <hyperlink ref="L71" r:id="rId106" xr:uid="{EB4C92E4-1242-4D64-91DF-0DE2E13E68FB}"/>
+    <hyperlink ref="L72" r:id="rId107" xr:uid="{2436ACB7-8CBE-4404-AB5D-6B4C22D775C3}"/>
+    <hyperlink ref="L75" r:id="rId108" xr:uid="{C4B27291-6EF3-4D11-8E80-4D291A6D89B6}"/>
+    <hyperlink ref="L76" r:id="rId109" xr:uid="{CE0B7581-A52B-4160-8992-25B0C5808961}"/>
+    <hyperlink ref="L77" r:id="rId110" xr:uid="{16AD970A-FACC-44EC-A1DA-25531A342731}"/>
+    <hyperlink ref="L79" r:id="rId111" xr:uid="{9D4B6EC4-19CB-4557-BE79-4136A2324550}"/>
+    <hyperlink ref="L80" r:id="rId112" xr:uid="{1A9BCA50-BE0C-4B22-A957-3B80712A2B17}"/>
+    <hyperlink ref="L81" r:id="rId113" xr:uid="{0DF291A6-D086-4CE4-B085-B94C715854AF}"/>
+    <hyperlink ref="L66" r:id="rId114" xr:uid="{868B7E99-AED5-4C00-8167-874AFB651830}"/>
+    <hyperlink ref="L68" r:id="rId115" xr:uid="{473DD8F3-5261-4CEC-A852-6CC3118CDF7E}"/>
+    <hyperlink ref="L70" r:id="rId116" xr:uid="{B4DA8F59-E30F-47C5-A54E-C36D8538B462}"/>
+    <hyperlink ref="L73" r:id="rId117" xr:uid="{08AA3B0B-5A39-4FE8-A037-B79F1B6732E0}"/>
+    <hyperlink ref="L74" r:id="rId118" xr:uid="{A4EEE11E-613B-4673-AB82-B49B140328D5}"/>
+    <hyperlink ref="L78" r:id="rId119" xr:uid="{F906F186-5393-4B72-B5FE-EA66A418B024}"/>
+    <hyperlink ref="U39" r:id="rId120" xr:uid="{26E6BED6-4A3F-4395-B762-09DAF12A3D17}"/>
+    <hyperlink ref="U41" r:id="rId121" xr:uid="{5B9D112A-2E91-4AB6-A662-AEFCF04E96B3}"/>
+    <hyperlink ref="L31" r:id="rId122" xr:uid="{22FEB9A6-CA72-443D-86AB-F6BBCE041DCC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId123"/>
@@ -13710,8 +13716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D633616-3BCA-4071-B84F-4B20AD4BC6F9}">
   <dimension ref="A1:Y53"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17988,6 +17994,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100764EA4CBCC3EB840B3A71EC084A37A79" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1c63f6b0f6065541758bb15ee54f6821">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9ed8ad31-4880-4d63-8f72-0ebd22f8068c" xmlns:ns4="819a0a68-6060-4071-a88e-471cccc4a5a4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0011b285b55bc13472d229a8f23f1c52" ns3:_="" ns4:_="">
     <xsd:import namespace="9ed8ad31-4880-4d63-8f72-0ebd22f8068c"/>
@@ -18204,22 +18225,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{538AE23B-FCFE-430C-92AD-3D09EEFD4655}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="819a0a68-6060-4071-a88e-471cccc4a5a4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="9ed8ad31-4880-4d63-8f72-0ebd22f8068c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAA63007-5F77-494C-AF11-EF28F74AE67F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6D1DAC1-61BB-432E-B17D-AB35AE99FFBA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18236,29 +18267,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{538AE23B-FCFE-430C-92AD-3D09EEFD4655}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="819a0a68-6060-4071-a88e-471cccc4a5a4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="9ed8ad31-4880-4d63-8f72-0ebd22f8068c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAA63007-5F77-494C-AF11-EF28F74AE67F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>